<commit_message>
Added data from Hawaii
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9888" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedSoil" sheetId="12" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -122,6 +122,24 @@
   </si>
   <si>
     <t>SubsurfaceMineralN</t>
+  </si>
+  <si>
+    <t>Gliricidia.AboveGround.Wt</t>
+  </si>
+  <si>
+    <t>Hamakuapoko</t>
+  </si>
+  <si>
+    <t>HamakuapokoCoppice</t>
+  </si>
+  <si>
+    <t>Gliricidia.Leaf.CoverGreen</t>
+  </si>
+  <si>
+    <t>StemsPerSqrM</t>
+  </si>
+  <si>
+    <t>Gliricidia.Leaf.LAI</t>
   </si>
 </sst>
 </file>
@@ -684,6 +702,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -968,11 +987,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242483512"/>
-        <c:axId val="242483904"/>
+        <c:axId val="3880104"/>
+        <c:axId val="238642488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242483512"/>
+        <c:axId val="3880104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,12 +1048,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242483904"/>
+        <c:crossAx val="238642488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242483904"/>
+        <c:axId val="238642488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242483512"/>
+        <c:crossAx val="3880104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1105,6 +1124,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1186,6 +1206,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1399,11 +1420,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242484688"/>
-        <c:axId val="242485080"/>
+        <c:axId val="238779880"/>
+        <c:axId val="238783056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242484688"/>
+        <c:axId val="238779880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,12 +1481,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242485080"/>
+        <c:crossAx val="238783056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242485080"/>
+        <c:axId val="238783056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1543,432 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242484688"/>
+        <c:crossAx val="238779880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ObservedGliricidia!$K$13:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.4229359211203001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5519769090135398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9641670285147903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2473239917054801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9534090444337906</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3154613715885803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.1720363768313895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.9463057989389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ObservedGliricidia!$I$13:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.26606850035580498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72551945440160492</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93499493915941401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97346174755908299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98127621581722591</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97848280861182702</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97802666996689391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98346674210044793</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ObservedGliricidia!$R$51:$R$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ObservedGliricidia!$S$51:$S$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45118836390597361</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59343034025940078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69880578808779781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77686983985157021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83470111177841344</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.87754357174701814</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90928204671058754</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93279448726025027</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="411291888"/>
+        <c:axId val="411291104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="411291888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411291104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="411291104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411291888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1651,6 +2097,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2683,20 +3169,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>179070</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>232410</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>483870</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>537210</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2717,16 +3719,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>240030</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>293370</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>544830</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>598170</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2740,6 +3742,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>461010</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3013,7 +4045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B50" sqref="B50:B65"/>
     </sheetView>
   </sheetViews>
@@ -3924,10 +4956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3937,7 +4969,7 @@
     <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3959,8 +4991,20 @@
       <c r="G1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3986,7 +5030,7 @@
         <v>279.06976744186045</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4008,11 +5052,11 @@
         <v>1.8</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="2">F3*1000/10/0.43</f>
+        <f t="shared" ref="G3:G11" si="2">F3*1000/10/0.43</f>
         <v>418.60465116279073</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4038,7 +5082,7 @@
         <v>395.34883720930236</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -4064,7 +5108,7 @@
         <v>511.62790697674421</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -4090,7 +5134,7 @@
         <v>558.1395348837209</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4116,7 +5160,7 @@
         <v>581.39534883720933</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -4142,7 +5186,7 @@
         <v>651.16279069767438</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -4168,7 +5212,7 @@
         <v>348.83720930232556</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4194,7 +5238,7 @@
         <v>488.37209302325584</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4220,7 +5264,7 @@
         <v>534.88372093023258</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4239,88 +5283,412 @@
         <v>491.35680000000002</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <f>YEAR(C13)</f>
+        <v>1988</v>
+      </c>
+      <c r="C13" s="3">
+        <v>32377</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>171.28653746087198</v>
+      </c>
+      <c r="I13">
+        <v>0.26606850035580498</v>
+      </c>
+      <c r="J13">
+        <v>1.27868852459016</v>
+      </c>
+      <c r="K13">
+        <v>1.4229359211203001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B28" si="3">YEAR(C14)</f>
+        <v>1988</v>
+      </c>
+      <c r="C14" s="3">
+        <v>32469</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>720.36696811434103</v>
+      </c>
+      <c r="I14">
+        <v>0.72551945440160492</v>
+      </c>
+      <c r="J14">
+        <v>1.4819672131147501</v>
+      </c>
+      <c r="K14">
+        <v>4.5519769090135398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C15" s="3">
+        <v>32561</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>1676.85443360362</v>
+      </c>
+      <c r="I15">
+        <v>0.93499493915941401</v>
+      </c>
+      <c r="J15">
+        <v>1.7442622950819602</v>
+      </c>
+      <c r="K15">
+        <v>6.9641670285147903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C16" s="3">
+        <v>32650</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>3018.5377059554498</v>
+      </c>
+      <c r="I16">
+        <v>0.97346174755908299</v>
+      </c>
+      <c r="J16">
+        <v>1.6590163934426201</v>
+      </c>
+      <c r="K16">
+        <v>9.2473239917054801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C17" s="3">
+        <v>32742</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>4434.2840107142101</v>
+      </c>
+      <c r="I17">
+        <v>0.98127621581722591</v>
+      </c>
+      <c r="J17">
+        <v>1.57377049180327</v>
+      </c>
+      <c r="K17">
+        <v>9.9534090444337906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C18" s="3">
+        <v>32834</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>5050.0145861777901</v>
+      </c>
+      <c r="I18">
+        <v>0.97848280861182702</v>
+      </c>
+      <c r="J18">
+        <v>1.46229508196721</v>
+      </c>
+      <c r="K18">
+        <v>6.3154613715885803</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="3"/>
+        <v>1990</v>
+      </c>
+      <c r="C19" s="3">
+        <v>32926</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>5495.3859210005203</v>
+      </c>
+      <c r="I19">
+        <v>0.97802666996689391</v>
+      </c>
+      <c r="J19">
+        <v>1.3049180327868801</v>
+      </c>
+      <c r="K19">
+        <v>9.1720363768313895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="3"/>
+        <v>1990</v>
+      </c>
+      <c r="C20" s="3">
+        <v>33015</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>5362.9470846391505</v>
+      </c>
+      <c r="I20">
+        <v>0.98346674210044793</v>
+      </c>
+      <c r="J20">
+        <v>1.28524590163934</v>
+      </c>
+      <c r="K20">
+        <v>12.9463057989389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="3"/>
+        <v>1988</v>
+      </c>
+      <c r="C21" s="3">
+        <v>32377</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>534.26014242328097</v>
+      </c>
+      <c r="I21">
+        <v>0.38280551786321998</v>
+      </c>
+      <c r="J21">
+        <v>4.4524590163934405</v>
+      </c>
+      <c r="K21">
+        <v>2.2831569631906898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="3"/>
+        <v>1988</v>
+      </c>
+      <c r="C22" s="3">
+        <v>32469</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>1416.6790885422101</v>
+      </c>
+      <c r="I22">
+        <v>0.86350139449362795</v>
+      </c>
+      <c r="J22">
+        <v>4.0852459016393396</v>
+      </c>
+      <c r="K22">
+        <v>6.8601740525742798</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C23" s="3">
+        <v>32561</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>2047.2354391994099</v>
+      </c>
+      <c r="I23">
+        <v>0.98099333913819808</v>
+      </c>
+      <c r="J23">
+        <v>3.5147540983606493</v>
+      </c>
+      <c r="K23">
+        <v>5.1720816259757898</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C24" s="3">
+        <v>32650</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>2107.38353234244</v>
+      </c>
+      <c r="I24">
+        <v>0.88148085941470999</v>
+      </c>
+      <c r="J24">
+        <v>3.1475409836065498</v>
+      </c>
+      <c r="K24">
+        <v>1.9354451341071499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C25" s="3">
+        <v>32742</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>2375.0046867812598</v>
+      </c>
+      <c r="I25">
+        <v>0.80320269440036696</v>
+      </c>
+      <c r="J25">
+        <v>2.97049180327868</v>
+      </c>
+      <c r="K25">
+        <v>6.0251707067481197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="3"/>
+        <v>1989</v>
+      </c>
+      <c r="C26" s="3">
+        <v>32834</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>2375.9264966378601</v>
+      </c>
+      <c r="I26">
+        <v>0.98083333701662301</v>
+      </c>
+      <c r="J26">
+        <v>2.9639344262295002</v>
+      </c>
+      <c r="K26">
+        <v>9.2974565629968104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="3"/>
+        <v>1990</v>
+      </c>
+      <c r="C27" s="3">
+        <v>32926</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="3"/>
+        <v>1990</v>
+      </c>
+      <c r="C28" s="3">
+        <v>33015</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
       <c r="F32" s="1"/>
     </row>
@@ -4375,6 +5743,92 @@
     <row r="45" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D45" s="2"/>
       <c r="F45" s="1"/>
+    </row>
+    <row r="50" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="S50">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="51" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <f>1-EXP(-S$50*R51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R52">
+        <v>2</v>
+      </c>
+      <c r="S52">
+        <f t="shared" ref="S52:S59" si="4">1-EXP(-S$50*R52)</f>
+        <v>0.45118836390597361</v>
+      </c>
+    </row>
+    <row r="53" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R53">
+        <v>3</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="4"/>
+        <v>0.59343034025940078</v>
+      </c>
+    </row>
+    <row r="54" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R54">
+        <v>4</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="4"/>
+        <v>0.69880578808779781</v>
+      </c>
+    </row>
+    <row r="55" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R55">
+        <v>5</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="4"/>
+        <v>0.77686983985157021</v>
+      </c>
+    </row>
+    <row r="56" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R56">
+        <v>6</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="4"/>
+        <v>0.83470111177841344</v>
+      </c>
+    </row>
+    <row r="57" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R57">
+        <v>7</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="4"/>
+        <v>0.87754357174701814</v>
+      </c>
+    </row>
+    <row r="58" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R58">
+        <v>8</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="4"/>
+        <v>0.90928204671058754</v>
+      </c>
+    </row>
+    <row r="59" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R59">
+        <v>9</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="4"/>
+        <v>0.93279448726025027</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed obs data for graphs
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Gliricidia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Gliricidia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,12 @@
     <sheet name="Akinnifesi 2006 Maize Yield" sheetId="2" r:id="rId4"/>
     <sheet name="C(%)" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="49">
   <si>
     <t>Year</t>
   </si>
@@ -159,11 +159,23 @@
   <si>
     <t>Gliricidia.Leaf.Detached.Wt</t>
   </si>
+  <si>
+    <t>MakokaN0MaizeSole</t>
+  </si>
+  <si>
+    <t>MakokaN48MaizeSole</t>
+  </si>
+  <si>
+    <t>MakokaN0MaizeGliricidia</t>
+  </si>
+  <si>
+    <t>MakokaN48MaizeGliricidia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,7 +718,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -876,7 +888,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C02B-49C3-9348-0B62844BE432}"/>
             </c:ext>
@@ -1000,7 +1012,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C02B-49C3-9348-0B62844BE432}"/>
             </c:ext>
@@ -1014,11 +1026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="3880104"/>
-        <c:axId val="238642488"/>
+        <c:axId val="233972192"/>
+        <c:axId val="235531616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3880104"/>
+        <c:axId val="233972192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,12 +1087,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238642488"/>
+        <c:crossAx val="235531616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238642488"/>
+        <c:axId val="235531616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,7 +1149,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3880104"/>
+        <c:crossAx val="233972192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1218,7 +1230,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1232,6 +1244,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1436,7 +1449,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C433-49FE-95A9-3FA2628AFC11}"/>
             </c:ext>
@@ -1450,11 +1463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238779880"/>
-        <c:axId val="238783056"/>
+        <c:axId val="235532400"/>
+        <c:axId val="235532792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238779880"/>
+        <c:axId val="235532400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1511,12 +1524,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238783056"/>
+        <c:crossAx val="235532792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238783056"/>
+        <c:axId val="235532792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238779880"/>
+        <c:crossAx val="235532400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1623,7 +1636,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1637,6 +1650,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1764,7 +1778,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EA7C-43B1-827B-6F0605D9D08F}"/>
             </c:ext>
@@ -1870,7 +1884,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EA7C-43B1-827B-6F0605D9D08F}"/>
             </c:ext>
@@ -1884,11 +1898,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="411291888"/>
-        <c:axId val="411291104"/>
+        <c:axId val="235533576"/>
+        <c:axId val="235533968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="411291888"/>
+        <c:axId val="235533576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,12 +1959,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411291104"/>
+        <c:crossAx val="235533968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="411291104"/>
+        <c:axId val="235533968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411291888"/>
+        <c:crossAx val="235533576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3895,23 +3909,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3947,23 +3944,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4118,18 +4098,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5234375" customWidth="1"/>
-    <col min="3" max="3" width="14.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4143,9 +4123,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4">
         <v>34991</v>
@@ -4155,9 +4135,9 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4">
         <v>35049</v>
@@ -4170,9 +4150,9 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4">
         <v>35082</v>
@@ -4185,9 +4165,9 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4">
         <v>35118</v>
@@ -4200,9 +4180,9 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4">
         <v>35139</v>
@@ -4215,9 +4195,9 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4">
         <v>35174</v>
@@ -4230,9 +4210,9 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B8" s="4">
         <v>35244</v>
@@ -4245,9 +4225,9 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4">
         <v>35307</v>
@@ -4260,9 +4240,9 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4">
         <v>35377</v>
@@ -4275,9 +4255,9 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B11" s="4">
         <v>35409</v>
@@ -4290,9 +4270,9 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4">
         <v>35074</v>
@@ -4305,9 +4285,9 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4">
         <v>35460</v>
@@ -4316,9 +4296,9 @@
         <v>9.0359999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4">
         <v>35489</v>
@@ -4331,9 +4311,9 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4">
         <v>35548</v>
@@ -4346,9 +4326,9 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4">
         <v>35649</v>
@@ -4361,9 +4341,9 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4">
         <v>35754</v>
@@ -4373,9 +4353,9 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4">
         <v>34991</v>
@@ -4385,9 +4365,9 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B19" s="4">
         <v>35049</v>
@@ -4399,9 +4379,9 @@
         <v>49.505000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4">
         <v>35082</v>
@@ -4413,9 +4393,9 @@
         <v>33.975000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4">
         <v>35118</v>
@@ -4427,9 +4407,9 @@
         <v>18.78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4">
         <v>35139</v>
@@ -4441,9 +4421,9 @@
         <v>23.655000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B23" s="4">
         <v>35174</v>
@@ -4455,9 +4435,9 @@
         <v>16.782</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4">
         <v>35244</v>
@@ -4469,9 +4449,9 @@
         <v>36.835000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B25" s="4">
         <v>35307</v>
@@ -4483,9 +4463,9 @@
         <v>49.939</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B26" s="4">
         <v>35377</v>
@@ -4497,9 +4477,9 @@
         <v>42.816000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B27" s="4">
         <v>35409</v>
@@ -4511,9 +4491,9 @@
         <v>27.969000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B28" s="4">
         <v>35074</v>
@@ -4525,9 +4505,9 @@
         <v>116.55500000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4">
         <v>35460</v>
@@ -4536,9 +4516,9 @@
         <v>5.7110000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B30" s="4">
         <v>35489</v>
@@ -4550,9 +4530,9 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4">
         <v>35548</v>
@@ -4564,9 +4544,9 @@
         <v>19.163</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B32" s="4">
         <v>35649</v>
@@ -4578,9 +4558,9 @@
         <v>41.692</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B33" s="4">
         <v>35754</v>
@@ -4590,9 +4570,9 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4">
         <v>34991</v>
@@ -4602,9 +4582,9 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B35" s="4">
         <v>35049</v>
@@ -4616,9 +4596,9 @@
         <v>33.709000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B36" s="4">
         <v>35082</v>
@@ -4630,9 +4610,9 @@
         <v>39.747999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B37" s="4">
         <v>35118</v>
@@ -4644,9 +4624,9 @@
         <v>13.172000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B38" s="4">
         <v>35139</v>
@@ -4658,9 +4638,9 @@
         <v>23.315999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B39" s="4">
         <v>35174</v>
@@ -4672,9 +4652,9 @@
         <v>17.97</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B40" s="4">
         <v>35244</v>
@@ -4686,9 +4666,9 @@
         <v>38.872999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4">
         <v>35307</v>
@@ -4700,9 +4680,9 @@
         <v>19.538</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B42" s="4">
         <v>35377</v>
@@ -4714,9 +4694,9 @@
         <v>33.136000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B43" s="4">
         <v>35409</v>
@@ -4728,9 +4708,9 @@
         <v>33.572000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B44" s="4">
         <v>35074</v>
@@ -4742,9 +4722,9 @@
         <v>98.212000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B45" s="4">
         <v>35460</v>
@@ -4753,9 +4733,9 @@
         <v>9.0370000000000008</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B46" s="4">
         <v>35489</v>
@@ -4767,9 +4747,9 @@
         <v>19.975999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B47" s="4">
         <v>35548</v>
@@ -4781,9 +4761,9 @@
         <v>22.559000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B48" s="4">
         <v>35649</v>
@@ -4795,9 +4775,9 @@
         <v>26.405999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B49" s="4">
         <v>35754</v>
@@ -4806,9 +4786,9 @@
         <v>95.965000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B50" s="4">
         <v>34991</v>
@@ -4817,9 +4797,9 @@
         <v>133.29599999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B51" s="4">
         <v>35049</v>
@@ -4831,9 +4811,9 @@
         <v>71.753</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B52" s="4">
         <v>35082</v>
@@ -4845,9 +4825,9 @@
         <v>41.109000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B53" s="4">
         <v>35118</v>
@@ -4859,9 +4839,9 @@
         <v>22.853999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B54" s="4">
         <v>35139</v>
@@ -4873,9 +4853,9 @@
         <v>27.902000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B55" s="4">
         <v>35174</v>
@@ -4887,9 +4867,9 @@
         <v>21.027999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B56" s="4">
         <v>35244</v>
@@ -4901,9 +4881,9 @@
         <v>37.171999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B57" s="4">
         <v>35307</v>
@@ -4915,9 +4895,9 @@
         <v>31.257000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B58" s="4">
         <v>35377</v>
@@ -4929,9 +4909,9 @@
         <v>40.438000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B59" s="4">
         <v>35409</v>
@@ -4943,9 +4923,9 @@
         <v>46.311</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B60" s="4">
         <v>35074</v>
@@ -4957,9 +4937,9 @@
         <v>94.135999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B61" s="4">
         <v>35460</v>
@@ -4968,9 +4948,9 @@
         <v>14.025</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B62" s="4">
         <v>35489</v>
@@ -4982,9 +4962,9 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B63" s="4">
         <v>35548</v>
@@ -4996,9 +4976,9 @@
         <v>15.596</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B64" s="4">
         <v>35649</v>
@@ -5010,9 +4990,9 @@
         <v>33.198999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B65" s="4">
         <v>35754</v>
@@ -5032,17 +5012,17 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5234375" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5086,7 +5066,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -5112,7 +5092,7 @@
         <v>279.06976744186045</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5138,7 +5118,7 @@
         <v>418.60465116279073</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5164,7 +5144,7 @@
         <v>395.34883720930236</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -5190,7 +5170,7 @@
         <v>511.62790697674421</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5216,7 +5196,7 @@
         <v>558.1395348837209</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5242,7 +5222,7 @@
         <v>581.39534883720933</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -5268,7 +5248,7 @@
         <v>651.16279069767438</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -5294,7 +5274,7 @@
         <v>348.83720930232556</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -5320,7 +5300,7 @@
         <v>488.37209302325584</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5346,7 +5326,7 @@
         <v>534.88372093023258</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -5366,7 +5346,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -5392,7 +5372,7 @@
         <v>1.4229359211203001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -5418,7 +5398,7 @@
         <v>4.5519769090135398</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -5444,7 +5424,7 @@
         <v>6.9641670285147903</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -5470,7 +5450,7 @@
         <v>9.2473239917054801</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -5496,7 +5476,7 @@
         <v>9.9534090444337906</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -5522,7 +5502,7 @@
         <v>6.3154613715885803</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -5548,7 +5528,7 @@
         <v>9.1720363768313895</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -5574,7 +5554,7 @@
         <v>12.9463057989389</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -5600,7 +5580,7 @@
         <v>2.2831569631906898</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -5626,7 +5606,7 @@
         <v>6.8601740525742798</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -5652,7 +5632,7 @@
         <v>5.1720816259757898</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -5678,7 +5658,7 @@
         <v>1.9354451341071499</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5704,7 +5684,7 @@
         <v>6.0251707067481197</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -5730,7 +5710,7 @@
         <v>9.2974565629968104</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -5744,7 +5724,7 @@
       <c r="D27" s="2"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -5758,7 +5738,7 @@
       <c r="D28" s="2"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -5781,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -5804,7 +5784,7 @@
         <v>47.948497854077509</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -5827,7 +5807,7 @@
         <v>333.34020028612167</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -5850,7 +5830,7 @@
         <v>500.90758226037059</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -5873,7 +5853,7 @@
         <v>289.82203147353323</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5896,7 +5876,7 @@
         <v>182.93333333333328</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5919,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -5942,12 +5922,12 @@
         <v>30.051293487956993</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="3">
-        <v>35290</v>
+        <v>35289</v>
       </c>
       <c r="D37" s="2"/>
       <c r="F37" s="1"/>
@@ -5965,7 +5945,7 @@
         <v>290.02230151650213</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -5985,7 +5965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -6008,7 +5988,7 @@
         <v>21.473015165030727</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6031,7 +6011,7 @@
         <v>191.12622658340734</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -6054,7 +6034,7 @@
         <v>296.57894736841979</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -6077,12 +6057,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="3">
-        <v>35236</v>
+        <v>35245</v>
       </c>
       <c r="D43" s="2"/>
       <c r="F43" s="1"/>
@@ -6100,7 +6080,7 @@
         <v>29.610912817612764</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -6120,7 +6100,7 @@
         <v>146.7248908296927</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -6143,12 +6123,12 @@
         <v>108.10580626921592</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="3">
-        <v>35290</v>
+        <v>35291</v>
       </c>
       <c r="H46">
         <f t="shared" si="4"/>
@@ -6161,12 +6141,12 @@
         <v>293.44978165938539</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>41</v>
       </c>
       <c r="C47" s="3">
-        <v>35348</v>
+        <v>35347</v>
       </c>
       <c r="H47">
         <f t="shared" si="4"/>
@@ -6182,7 +6162,7 @@
         <v>84.832667773968865</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -6200,12 +6180,12 @@
         <v>146.7248908296927</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>41</v>
       </c>
       <c r="C49" s="3">
-        <v>35400</v>
+        <v>35399</v>
       </c>
       <c r="H49">
         <f t="shared" si="4"/>
@@ -6221,7 +6201,7 @@
         <v>61.351733399300393</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -6242,7 +6222,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -6270,7 +6250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R52">
         <v>2</v>
       </c>
@@ -6279,7 +6259,7 @@
         <v>0.45118836390597361</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R53">
         <v>3</v>
       </c>
@@ -6288,7 +6268,7 @@
         <v>0.59343034025940078</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R54">
         <v>4</v>
       </c>
@@ -6297,7 +6277,7 @@
         <v>0.69880578808779781</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R55">
         <v>5</v>
       </c>
@@ -6306,7 +6286,7 @@
         <v>0.77686983985157021</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R56">
         <v>6</v>
       </c>
@@ -6315,7 +6295,7 @@
         <v>0.83470111177841344</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R57">
         <v>7</v>
       </c>
@@ -6324,7 +6304,7 @@
         <v>0.87754357174701814</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R58">
         <v>8</v>
       </c>
@@ -6333,7 +6313,7 @@
         <v>0.90928204671058754</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R59">
         <v>9</v>
       </c>
@@ -6357,12 +6337,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5234375" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6379,7 +6359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -6397,7 +6377,7 @@
         <v>348.33299999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -6409,7 +6389,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -6427,7 +6407,7 @@
         <v>458.88900000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -6439,7 +6419,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -6457,7 +6437,7 @@
         <v>820.55600000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -6469,7 +6449,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -6487,7 +6467,7 @@
         <v>330.55600000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -6499,7 +6479,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -6517,7 +6497,7 @@
         <v>627.22199999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -6529,7 +6509,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -6547,7 +6527,7 @@
         <v>326.11099999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -6559,7 +6539,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -6577,7 +6557,7 @@
         <v>1133.3330000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -6589,7 +6569,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -6607,7 +6587,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -6619,7 +6599,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -6637,7 +6617,7 @@
         <v>717.22199999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -6649,7 +6629,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -6667,7 +6647,7 @@
         <v>132.77799999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -6679,7 +6659,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -6697,7 +6677,7 @@
         <v>910.55600000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -6709,7 +6689,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -6727,7 +6707,7 @@
         <v>240.55599999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -6739,7 +6719,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -6757,7 +6737,7 @@
         <v>953.33300000000008</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -6769,7 +6749,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -6787,7 +6767,7 @@
         <v>227.22199999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -6799,7 +6779,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -6817,7 +6797,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -6829,7 +6809,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -6847,7 +6827,7 @@
         <v>184.44400000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -6859,7 +6839,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -6877,7 +6857,7 @@
         <v>1081.6669999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -6889,7 +6869,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -6907,7 +6887,7 @@
         <v>193.333</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -6919,7 +6899,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -6937,7 +6917,7 @@
         <v>892.77800000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -6949,7 +6929,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -6967,7 +6947,7 @@
         <v>202.22199999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -6979,7 +6959,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -6991,7 +6971,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -7003,7 +6983,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -7015,7 +6995,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -7041,13 +7021,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.1015625" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7058,7 +7038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -7069,7 +7049,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -7080,7 +7060,7 @@
         <v>3922</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -7091,7 +7071,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -7102,7 +7082,7 @@
         <v>5302</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1997</v>
       </c>
@@ -7113,7 +7093,7 @@
         <v>3356</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1998</v>
       </c>
@@ -7124,7 +7104,7 @@
         <v>4322</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1999</v>
       </c>
@@ -7135,7 +7115,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2000</v>
       </c>
@@ -7146,7 +7126,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -7157,7 +7137,7 @@
         <v>5059</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -7181,13 +7161,13 @@
       <selection activeCell="A48" sqref="A47:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.89453125" customWidth="1"/>
-    <col min="2" max="2" width="11.1015625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7198,7 +7178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7209,7 +7189,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -7220,7 +7200,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -7231,7 +7211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -7242,7 +7222,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7253,7 +7233,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7264,7 +7244,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -7275,7 +7255,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -7286,7 +7266,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -7297,7 +7277,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -7308,7 +7288,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -7319,7 +7299,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -7330,7 +7310,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -7341,7 +7321,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -7352,7 +7332,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -7363,7 +7343,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -7374,7 +7354,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -7385,7 +7365,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -7396,7 +7376,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -7407,7 +7387,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Updated Makoka maize data
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9888" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9888" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedSoil" sheetId="12" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -77,18 +77,6 @@
   </si>
   <si>
     <t>80-100</t>
-  </si>
-  <si>
-    <t>Gm</t>
-  </si>
-  <si>
-    <t>Gm48N</t>
-  </si>
-  <si>
-    <t>MakokaN0</t>
-  </si>
-  <si>
-    <t>MakokaN48</t>
   </si>
   <si>
     <t>MakokaGliricidiaBase</t>
@@ -171,11 +159,30 @@
   <si>
     <t>MakokaN48MaizeGliricidia</t>
   </si>
+  <si>
+    <t>MakokaN24MaizeSole</t>
+  </si>
+  <si>
+    <t>MakokaN24MaizeGliricidia</t>
+  </si>
+  <si>
+    <t>Thouseed</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>%standloss</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,12 +660,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,11 +1035,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233972192"/>
-        <c:axId val="235531616"/>
+        <c:axId val="241752208"/>
+        <c:axId val="241752600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233972192"/>
+        <c:axId val="241752208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,12 +1096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235531616"/>
+        <c:crossAx val="241752600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235531616"/>
+        <c:axId val="241752600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233972192"/>
+        <c:crossAx val="241752208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1244,7 +1253,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1463,11 +1471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235532400"/>
-        <c:axId val="235532792"/>
+        <c:axId val="241753384"/>
+        <c:axId val="241753776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235532400"/>
+        <c:axId val="241753384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,12 +1532,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235532792"/>
+        <c:crossAx val="241753776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235532792"/>
+        <c:axId val="241753776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235532400"/>
+        <c:crossAx val="241753384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1650,7 +1658,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1898,11 +1905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235533576"/>
-        <c:axId val="235533968"/>
+        <c:axId val="241754560"/>
+        <c:axId val="241754952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235533576"/>
+        <c:axId val="241754560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,12 +1966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235533968"/>
+        <c:crossAx val="241754952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235533968"/>
+        <c:axId val="241754952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2021,7 +2028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235533576"/>
+        <c:crossAx val="241754560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4114,18 +4121,18 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4">
         <v>34991</v>
@@ -4137,7 +4144,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4">
         <v>35049</v>
@@ -4152,7 +4159,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4">
         <v>35082</v>
@@ -4167,7 +4174,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4">
         <v>35118</v>
@@ -4182,7 +4189,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4">
         <v>35139</v>
@@ -4197,7 +4204,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4">
         <v>35174</v>
@@ -4212,7 +4219,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4">
         <v>35244</v>
@@ -4227,7 +4234,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4">
         <v>35307</v>
@@ -4242,7 +4249,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4">
         <v>35377</v>
@@ -4257,7 +4264,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4">
         <v>35409</v>
@@ -4272,7 +4279,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="4">
         <v>35074</v>
@@ -4287,7 +4294,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
         <v>35460</v>
@@ -4298,7 +4305,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>35489</v>
@@ -4313,7 +4320,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4">
         <v>35548</v>
@@ -4328,7 +4335,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4">
         <v>35649</v>
@@ -4343,7 +4350,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4">
         <v>35754</v>
@@ -4355,7 +4362,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4">
         <v>34991</v>
@@ -4367,7 +4374,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4">
         <v>35049</v>
@@ -4381,7 +4388,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4">
         <v>35082</v>
@@ -4395,7 +4402,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4">
         <v>35118</v>
@@ -4409,7 +4416,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4">
         <v>35139</v>
@@ -4423,7 +4430,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B23" s="4">
         <v>35174</v>
@@ -4437,7 +4444,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" s="4">
         <v>35244</v>
@@ -4451,7 +4458,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B25" s="4">
         <v>35307</v>
@@ -4465,7 +4472,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="4">
         <v>35377</v>
@@ -4479,7 +4486,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B27" s="4">
         <v>35409</v>
@@ -4493,7 +4500,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B28" s="4">
         <v>35074</v>
@@ -4507,7 +4514,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B29" s="4">
         <v>35460</v>
@@ -4518,7 +4525,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B30" s="4">
         <v>35489</v>
@@ -4532,7 +4539,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B31" s="4">
         <v>35548</v>
@@ -4546,7 +4553,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B32" s="4">
         <v>35649</v>
@@ -4560,7 +4567,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B33" s="4">
         <v>35754</v>
@@ -4572,7 +4579,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="4">
         <v>34991</v>
@@ -4584,7 +4591,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4">
         <v>35049</v>
@@ -4598,7 +4605,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B36" s="4">
         <v>35082</v>
@@ -4612,7 +4619,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4">
         <v>35118</v>
@@ -4626,7 +4633,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" s="4">
         <v>35139</v>
@@ -4640,7 +4647,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B39" s="4">
         <v>35174</v>
@@ -4654,7 +4661,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B40" s="4">
         <v>35244</v>
@@ -4668,7 +4675,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B41" s="4">
         <v>35307</v>
@@ -4682,7 +4689,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4">
         <v>35377</v>
@@ -4696,7 +4703,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B43" s="4">
         <v>35409</v>
@@ -4710,7 +4717,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4">
         <v>35074</v>
@@ -4724,7 +4731,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B45" s="4">
         <v>35460</v>
@@ -4735,7 +4742,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B46" s="4">
         <v>35489</v>
@@ -4749,7 +4756,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B47" s="4">
         <v>35548</v>
@@ -4763,7 +4770,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B48" s="4">
         <v>35649</v>
@@ -4777,7 +4784,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B49" s="4">
         <v>35754</v>
@@ -4788,7 +4795,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B50" s="4">
         <v>34991</v>
@@ -4799,7 +4806,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B51" s="4">
         <v>35049</v>
@@ -4813,7 +4820,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B52" s="4">
         <v>35082</v>
@@ -4827,7 +4834,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B53" s="4">
         <v>35118</v>
@@ -4841,7 +4848,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B54" s="4">
         <v>35139</v>
@@ -4855,7 +4862,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B55" s="4">
         <v>35174</v>
@@ -4869,7 +4876,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B56" s="4">
         <v>35244</v>
@@ -4883,7 +4890,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B57" s="4">
         <v>35307</v>
@@ -4897,7 +4904,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B58" s="4">
         <v>35377</v>
@@ -4911,7 +4918,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B59" s="4">
         <v>35409</v>
@@ -4925,7 +4932,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B60" s="4">
         <v>35074</v>
@@ -4939,7 +4946,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B61" s="4">
         <v>35460</v>
@@ -4950,7 +4957,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B62" s="4">
         <v>35489</v>
@@ -4964,7 +4971,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B63" s="4">
         <v>35548</v>
@@ -4978,7 +4985,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B64" s="4">
         <v>35649</v>
@@ -4992,7 +4999,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B65" s="4">
         <v>35754</v>
@@ -5011,8 +5018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5030,45 +5037,45 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
       <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1993</v>
@@ -5094,7 +5101,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>1994</v>
@@ -5120,7 +5127,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1995</v>
@@ -5146,7 +5153,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1996</v>
@@ -5172,7 +5179,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>1997</v>
@@ -5198,7 +5205,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1998</v>
@@ -5224,7 +5231,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>1999</v>
@@ -5250,7 +5257,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>2000</v>
@@ -5276,7 +5283,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>2001</v>
@@ -5302,7 +5309,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>2002</v>
@@ -5328,7 +5335,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2003</v>
@@ -5348,7 +5355,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <f>YEAR(C13)</f>
@@ -5374,7 +5381,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B28" si="3">YEAR(C14)</f>
@@ -5400,7 +5407,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <f t="shared" si="3"/>
@@ -5426,7 +5433,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <f t="shared" si="3"/>
@@ -5452,7 +5459,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <f t="shared" si="3"/>
@@ -5478,7 +5485,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <f t="shared" si="3"/>
@@ -5504,7 +5511,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <f t="shared" si="3"/>
@@ -5530,7 +5537,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <f t="shared" si="3"/>
@@ -5556,7 +5563,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <f t="shared" si="3"/>
@@ -5582,7 +5589,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B22">
         <f t="shared" si="3"/>
@@ -5608,7 +5615,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <f t="shared" si="3"/>
@@ -5634,7 +5641,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <f t="shared" si="3"/>
@@ -5660,7 +5667,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <f t="shared" si="3"/>
@@ -5686,7 +5693,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <f t="shared" si="3"/>
@@ -5712,7 +5719,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <f t="shared" si="3"/>
@@ -5726,7 +5733,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <f t="shared" si="3"/>
@@ -5740,7 +5747,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="3">
         <v>35184</v>
@@ -5763,7 +5770,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3">
         <v>35236</v>
@@ -5786,7 +5793,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C31" s="3">
         <v>35290</v>
@@ -5809,7 +5816,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3">
         <v>35348</v>
@@ -5832,7 +5839,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C33" s="3">
         <v>35400</v>
@@ -5855,7 +5862,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C34" s="3">
         <v>35461</v>
@@ -5878,7 +5885,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C35" s="3">
         <v>35184</v>
@@ -5901,7 +5908,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C36" s="3">
         <v>35236</v>
@@ -5924,7 +5931,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37" s="3">
         <v>35289</v>
@@ -5947,7 +5954,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3">
         <v>35290</v>
@@ -5967,7 +5974,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3">
         <v>35348</v>
@@ -5990,7 +5997,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C40" s="3">
         <v>35400</v>
@@ -6013,7 +6020,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3">
         <v>35461</v>
@@ -6036,7 +6043,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C42" s="3">
         <v>35184</v>
@@ -6059,7 +6066,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3">
         <v>35245</v>
@@ -6082,7 +6089,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C44" s="3">
         <v>35236</v>
@@ -6102,7 +6109,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C45" s="3">
         <v>35290</v>
@@ -6125,7 +6132,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C46" s="3">
         <v>35291</v>
@@ -6143,7 +6150,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C47" s="3">
         <v>35347</v>
@@ -6164,7 +6171,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C48" s="3">
         <v>35348</v>
@@ -6182,7 +6189,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C49" s="3">
         <v>35399</v>
@@ -6203,7 +6210,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C50" s="3">
         <v>35400</v>
@@ -6224,7 +6231,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C51" s="3">
         <v>35461</v>
@@ -6331,10 +6338,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6342,7 +6349,7 @@
     <col min="1" max="1" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6350,662 +6357,1655 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2">
         <v>1993</v>
       </c>
-      <c r="C2" s="2">
-        <v>173.333</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="5">
+        <v>199.4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>250</v>
+      </c>
+      <c r="E2" s="5">
+        <v>449.4</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.44370271473075212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1993</v>
+      </c>
+      <c r="C3" s="5">
+        <v>341.8</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1993</v>
+      </c>
+      <c r="C4" s="5">
+        <v>414.7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1993</v>
+      </c>
+      <c r="C5" s="5">
+        <v>165.7</v>
+      </c>
+      <c r="D5" s="5">
         <v>175</v>
       </c>
-      <c r="E2" s="1">
-        <f>C2+D2</f>
-        <v>348.33299999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
+      <c r="E5" s="5">
+        <v>340.7</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.48635162899911943</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2">
         <v>1993</v>
       </c>
-      <c r="C3" s="2">
-        <v>408.88900000000001</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
+      <c r="C6" s="5">
+        <v>298.2</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2">
         <v>1993</v>
       </c>
-      <c r="C4" s="2">
-        <v>208.88900000000001</v>
-      </c>
-      <c r="D4">
-        <v>250</v>
-      </c>
-      <c r="E4" s="1">
-        <f>C4+D4</f>
-        <v>458.88900000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>1993</v>
-      </c>
-      <c r="C5" s="2">
-        <v>408.88900000000001</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
+      <c r="C7" s="5">
+        <v>401.3</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2">
         <v>1994</v>
       </c>
-      <c r="C6" s="2">
-        <v>395.55599999999998</v>
-      </c>
-      <c r="D6">
+      <c r="C8" s="5">
+        <v>150.1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>175</v>
+      </c>
+      <c r="E8" s="5">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.46170409104890797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1994</v>
+      </c>
+      <c r="C9" s="5">
+        <v>211.1</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1994</v>
+      </c>
+      <c r="C10" s="5">
+        <v>315.5</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1994</v>
+      </c>
+      <c r="C11" s="5">
+        <v>392.2</v>
+      </c>
+      <c r="D11" s="5">
         <v>425</v>
       </c>
-      <c r="E6" s="1">
-        <f>C6+D6</f>
-        <v>820.55600000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
+      <c r="E11" s="5">
+        <v>817.2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.47993147332354374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2">
         <v>1994</v>
       </c>
-      <c r="C7" s="2">
-        <v>462.22199999999998</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
+      <c r="C12" s="5">
+        <v>444.6</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2">
         <v>1994</v>
       </c>
-      <c r="C8" s="2">
-        <v>155.55600000000001</v>
-      </c>
-      <c r="D8">
+      <c r="C13" s="5">
+        <v>454.4</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C14" s="5">
+        <v>149</v>
+      </c>
+      <c r="D14" s="5">
         <v>175</v>
       </c>
-      <c r="E8" s="1">
-        <f>C8+D8</f>
-        <v>330.55600000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>1994</v>
-      </c>
-      <c r="C9" s="2">
-        <v>320</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
+      <c r="E14" s="5">
+        <v>324</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.45987654320987653</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2">
         <v>1995</v>
       </c>
-      <c r="C10" s="2">
-        <v>302.22199999999998</v>
-      </c>
-      <c r="D10">
+      <c r="C15" s="5">
+        <v>310.8</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C16" s="5">
+        <v>332</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C17" s="5">
+        <v>298.39999999999998</v>
+      </c>
+      <c r="D17" s="5">
         <v>325</v>
       </c>
-      <c r="E10" s="1">
-        <f>C10+D10</f>
-        <v>627.22199999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
+      <c r="E17" s="5">
+        <v>623.4</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.47866538338145653</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2">
         <v>1995</v>
       </c>
-      <c r="C11" s="2">
-        <v>382.22199999999998</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12">
+      <c r="C18" s="5">
+        <v>409.2</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="2">
         <v>1995</v>
       </c>
-      <c r="C12" s="2">
-        <v>151.11099999999999</v>
-      </c>
-      <c r="D12">
-        <v>175</v>
-      </c>
-      <c r="E12" s="1">
-        <f>C12+D12</f>
-        <v>326.11099999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>1995</v>
-      </c>
-      <c r="C13" s="2">
-        <v>342.22199999999998</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
+      <c r="C19" s="5">
+        <v>373</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2">
         <v>1996</v>
       </c>
-      <c r="C14" s="2">
-        <v>533.33299999999997</v>
-      </c>
-      <c r="D14">
+      <c r="C20" s="5">
+        <v>120</v>
+      </c>
+      <c r="D20" s="5">
+        <v>150</v>
+      </c>
+      <c r="E20" s="5">
+        <v>270</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C21" s="5">
+        <v>391.7</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C22" s="5">
+        <v>475</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C23" s="5">
+        <v>530.20000000000005</v>
+      </c>
+      <c r="D23" s="5">
         <v>600</v>
       </c>
-      <c r="E14" s="1">
-        <f>C14+D14</f>
-        <v>1133.3330000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
+      <c r="E23" s="5">
+        <v>1130.2</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.46912050964431079</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2">
         <v>1996</v>
       </c>
-      <c r="C15" s="2">
-        <v>755.55600000000004</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
+      <c r="C24" s="5">
+        <v>409.2</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2">
         <v>1996</v>
       </c>
-      <c r="C16" s="2">
-        <v>120</v>
-      </c>
-      <c r="D16">
-        <v>150</v>
-      </c>
-      <c r="E16" s="1">
-        <f>C16+D16</f>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>1996</v>
-      </c>
-      <c r="C17" s="2">
-        <v>480</v>
-      </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
+      <c r="C25" s="5">
+        <v>752.3</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2">
         <v>1997</v>
       </c>
-      <c r="C18" s="2">
-        <v>342.22199999999998</v>
-      </c>
-      <c r="D18">
+      <c r="C26" s="5">
+        <v>52.9</v>
+      </c>
+      <c r="D26" s="5">
+        <v>75</v>
+      </c>
+      <c r="E26" s="5">
+        <v>127.9</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.41360437842064107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1997</v>
+      </c>
+      <c r="C27" s="5">
+        <v>198.7</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1997</v>
+      </c>
+      <c r="C28" s="5">
+        <v>193.1</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1997</v>
+      </c>
+      <c r="C29" s="5">
+        <v>335.6</v>
+      </c>
+      <c r="D29" s="5">
         <v>375</v>
       </c>
-      <c r="E18" s="1">
-        <f>C18+D18</f>
-        <v>717.22199999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
+      <c r="E29" s="5">
+        <v>710.6</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.47227694905713485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="2">
         <v>1997</v>
       </c>
-      <c r="C19" s="2">
-        <v>453.33300000000003</v>
-      </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
+      <c r="C30" s="5">
+        <v>416</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2">
         <v>1997</v>
       </c>
-      <c r="C20" s="2">
-        <v>57.777999999999999</v>
-      </c>
-      <c r="D20">
-        <v>75</v>
-      </c>
-      <c r="E20" s="1">
-        <f>C20+D20</f>
-        <v>132.77799999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>1997</v>
-      </c>
-      <c r="C21" s="2">
-        <v>195.55600000000001</v>
-      </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
+      <c r="C31" s="5">
+        <v>446.9</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="2">
         <v>1998</v>
       </c>
-      <c r="C22" s="2">
-        <v>435.55599999999998</v>
-      </c>
-      <c r="D22">
+      <c r="C32" s="5">
+        <v>107.3</v>
+      </c>
+      <c r="D32" s="5">
+        <v>125</v>
+      </c>
+      <c r="E32" s="5">
+        <v>232.3</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.46190271201033145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1998</v>
+      </c>
+      <c r="C33" s="5">
+        <v>295.3</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1998</v>
+      </c>
+      <c r="C34" s="5">
+        <v>400</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1998</v>
+      </c>
+      <c r="C35" s="5">
+        <v>432.2</v>
+      </c>
+      <c r="D35" s="5">
         <v>475</v>
       </c>
-      <c r="E22" s="1">
-        <f>C22+D22</f>
-        <v>910.55600000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23">
+      <c r="E35" s="5">
+        <v>907.2</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.47641093474426804</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2">
         <v>1998</v>
       </c>
-      <c r="C23" s="2">
-        <v>586.66700000000003</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24">
+      <c r="C36" s="5">
+        <v>599.70000000000005</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="2">
         <v>1998</v>
       </c>
-      <c r="C24" s="2">
-        <v>115.556</v>
-      </c>
-      <c r="D24">
+      <c r="C37" s="5">
+        <v>581.5</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C38" s="5">
+        <v>101.5</v>
+      </c>
+      <c r="D38" s="5">
         <v>125</v>
       </c>
-      <c r="E24" s="1">
-        <f>C24+D24</f>
-        <v>240.55599999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>1998</v>
-      </c>
-      <c r="C25" s="2">
-        <v>404.44400000000002</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26">
+      <c r="E38" s="5">
+        <v>226.5</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="6">
+        <v>0.44812362030905079</v>
+      </c>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="2">
         <v>1999</v>
       </c>
-      <c r="C26" s="2">
-        <v>453.33300000000003</v>
-      </c>
-      <c r="D26">
+      <c r="C39" s="5">
+        <v>264.60000000000002</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C40" s="5">
+        <v>384.4</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C41" s="5">
+        <v>448.7</v>
+      </c>
+      <c r="D41" s="5">
         <v>500</v>
       </c>
-      <c r="E26" s="1">
-        <f>C26+D26</f>
-        <v>953.33300000000008</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27">
+      <c r="E41" s="5">
+        <v>948.7</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="6">
+        <v>0.47296300200274055</v>
+      </c>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="2">
         <v>1999</v>
       </c>
-      <c r="C27" s="2">
-        <v>648.88900000000001</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28">
+      <c r="C42" s="5">
+        <v>592.6</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2">
         <v>1999</v>
       </c>
-      <c r="C28" s="2">
-        <v>102.22199999999999</v>
-      </c>
-      <c r="D28">
-        <v>125</v>
-      </c>
-      <c r="E28" s="1">
-        <f>C28+D28</f>
-        <v>227.22199999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29">
-        <v>1999</v>
-      </c>
-      <c r="C29" s="2">
-        <v>391.11099999999999</v>
-      </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30">
+      <c r="C43" s="5">
+        <v>645.5</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="2">
         <v>2000</v>
       </c>
-      <c r="C30" s="2">
-        <v>240</v>
-      </c>
-      <c r="D30">
+      <c r="C44" s="5">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D44" s="5">
+        <v>100</v>
+      </c>
+      <c r="E44" s="5">
+        <v>180.4</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="6">
+        <v>0.44567627494456763</v>
+      </c>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C45" s="5">
+        <v>170.8</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C46" s="5">
+        <v>207.6</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C47" s="5">
+        <v>230.9</v>
+      </c>
+      <c r="D47" s="5">
         <v>275</v>
       </c>
-      <c r="E30" s="1">
-        <f>C30+D30</f>
-        <v>515</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31">
+      <c r="E47" s="5">
+        <v>505.9</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="6">
+        <v>0.45641431112868158</v>
+      </c>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2">
         <v>2000</v>
       </c>
-      <c r="C31" s="2">
-        <v>360</v>
-      </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32">
+      <c r="C48" s="5">
+        <v>294.7</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2">
         <v>2000</v>
       </c>
-      <c r="C32" s="2">
-        <v>84.444000000000003</v>
-      </c>
-      <c r="D32">
+      <c r="C49" s="5">
+        <v>351.9</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2001</v>
+      </c>
+      <c r="C50" s="5">
+        <v>85.7</v>
+      </c>
+      <c r="D50" s="5">
         <v>100</v>
       </c>
-      <c r="E32" s="1">
-        <f>C32+D32</f>
-        <v>184.44400000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33">
-        <v>2000</v>
-      </c>
-      <c r="C33" s="2">
-        <v>217.77799999999999</v>
-      </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34">
+      <c r="E50" s="5">
+        <v>185.7</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="6">
+        <v>0.46149703823371035</v>
+      </c>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2">
         <v>2001</v>
       </c>
-      <c r="C34" s="2">
-        <v>506.66699999999997</v>
-      </c>
-      <c r="D34">
+      <c r="C51" s="5">
+        <v>264</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2001</v>
+      </c>
+      <c r="C52" s="5">
+        <v>301.8</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2001</v>
+      </c>
+      <c r="C53" s="5">
+        <v>505.9</v>
+      </c>
+      <c r="D53" s="5">
         <v>575</v>
       </c>
-      <c r="E34" s="1">
-        <f>C34+D34</f>
-        <v>1081.6669999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35">
+      <c r="E53" s="5">
+        <v>1080.9000000000001</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="6">
+        <v>0.46803589601258205</v>
+      </c>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="2">
         <v>2001</v>
       </c>
-      <c r="C35" s="2">
-        <v>640</v>
-      </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36">
+      <c r="C54" s="5">
+        <v>583</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="2">
         <v>2001</v>
       </c>
-      <c r="C36" s="2">
-        <v>93.332999999999998</v>
-      </c>
-      <c r="D36">
+      <c r="C55" s="5">
+        <v>634.4</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C56" s="5">
         <v>100</v>
       </c>
-      <c r="E36" s="1">
-        <f>C36+D36</f>
-        <v>193.333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37">
-        <v>2001</v>
-      </c>
-      <c r="C37" s="2">
-        <v>302.22199999999998</v>
-      </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38">
+      <c r="D56" s="5">
+        <v>100</v>
+      </c>
+      <c r="E56" s="5">
+        <v>200</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="2">
         <v>2002</v>
       </c>
-      <c r="C38" s="2">
-        <v>417.77800000000002</v>
-      </c>
-      <c r="D38">
+      <c r="C57" s="5">
+        <v>289</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C58" s="5">
+        <v>362</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C59" s="5">
+        <v>415</v>
+      </c>
+      <c r="D59" s="5">
         <v>475</v>
       </c>
-      <c r="E38" s="1">
-        <f>C38+D38</f>
-        <v>892.77800000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39">
+      <c r="E59" s="5">
+        <v>890</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="6">
+        <v>0.46629213483146065</v>
+      </c>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="2">
         <v>2002</v>
       </c>
-      <c r="C39" s="2">
-        <v>520</v>
-      </c>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40">
+      <c r="C60" s="5">
+        <v>529</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="2">
         <v>2002</v>
       </c>
-      <c r="C40" s="2">
-        <v>102.22199999999999</v>
-      </c>
-      <c r="D40">
-        <v>100</v>
-      </c>
-      <c r="E40" s="1">
-        <f>C40+D40</f>
-        <v>202.22199999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41">
-        <v>2002</v>
-      </c>
-      <c r="C41" s="2">
-        <v>364.44400000000002</v>
-      </c>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42">
+      <c r="C61" s="5">
+        <v>512</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="2">
         <v>2003</v>
       </c>
-      <c r="C42" s="2">
-        <v>404.44400000000002</v>
-      </c>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43">
+      <c r="C62" s="5">
+        <v>147.73756097560974</v>
+      </c>
+      <c r="D62" s="5">
+        <v>155.55911725805495</v>
+      </c>
+      <c r="E62" s="5">
+        <v>303.29667823366469</v>
+      </c>
+      <c r="F62" s="2">
+        <v>311.11666666666662</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0.48834578500969578</v>
+      </c>
+      <c r="H62" s="1">
+        <v>20.174684645498044</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="2">
         <v>2003</v>
       </c>
-      <c r="C43" s="2">
-        <v>520</v>
-      </c>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44">
+      <c r="C63" s="5">
+        <v>325.54268292682929</v>
+      </c>
+      <c r="D63" s="5">
+        <v>369.85980564972425</v>
+      </c>
+      <c r="E63" s="5">
+        <v>695.40248857655354</v>
+      </c>
+      <c r="F63" s="2">
+        <v>377.26333333333332</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0.46296529638549005</v>
+      </c>
+      <c r="H63" s="1">
+        <v>12.614615807812214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="2">
         <v>2003</v>
       </c>
-      <c r="C44" s="2">
-        <v>120</v>
-      </c>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45">
+      <c r="C64" s="5">
+        <v>288.6708943089431</v>
+      </c>
+      <c r="D64" s="5">
+        <v>295.01782089694558</v>
+      </c>
+      <c r="E64" s="5">
+        <v>583.68871520588868</v>
+      </c>
+      <c r="F64" s="2">
+        <v>330.28</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0.49304866218202514</v>
+      </c>
+      <c r="H64" s="1">
+        <v>10.2986955631914</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="2">
         <v>2003</v>
       </c>
-      <c r="C45" s="2">
-        <v>360</v>
-      </c>
-      <c r="E45" s="1"/>
+      <c r="C65" s="5">
+        <v>491.48411382113829</v>
+      </c>
+      <c r="D65" s="5">
+        <v>482.88396143730677</v>
+      </c>
+      <c r="E65" s="5">
+        <v>974.36807525844506</v>
+      </c>
+      <c r="F65" s="2">
+        <v>412.77500000000003</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0.50308413969094035</v>
+      </c>
+      <c r="H65" s="1">
+        <v>17.604570573283841</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C66" s="5">
+        <v>566.48069105691059</v>
+      </c>
+      <c r="D66" s="5">
+        <v>576.54709782611837</v>
+      </c>
+      <c r="E66" s="5">
+        <v>1143.027788883029</v>
+      </c>
+      <c r="F66" s="2">
+        <v>418.03</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0.49478288809734661</v>
+      </c>
+      <c r="H66" s="1">
+        <v>15.271238981895833</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C67" s="5">
+        <v>500.80959349593502</v>
+      </c>
+      <c r="D67" s="5">
+        <v>567.31906756528008</v>
+      </c>
+      <c r="E67" s="5">
+        <v>1068.1286610612151</v>
+      </c>
+      <c r="F67" s="2">
+        <v>388.0116666666666</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0.47731697382290128</v>
+      </c>
+      <c r="H67" s="1">
+        <v>16.095937452239973</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C68" s="5">
+        <v>109.05594995833671</v>
+      </c>
+      <c r="D68" s="5">
+        <v>166.40384123662309</v>
+      </c>
+      <c r="E68" s="5">
+        <v>275.45979119495979</v>
+      </c>
+      <c r="F68" s="2">
+        <v>297.19666666666666</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0.39853687851550257</v>
+      </c>
+      <c r="H68" s="1">
+        <v>2.035973976272484</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C69" s="5">
+        <v>318.76249839404187</v>
+      </c>
+      <c r="D69" s="5">
+        <v>307.48270734493406</v>
+      </c>
+      <c r="E69" s="5">
+        <v>626.24520573897598</v>
+      </c>
+      <c r="F69" s="2">
+        <v>348.52333333333331</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0.50808374593232708</v>
+      </c>
+      <c r="H69" s="1">
+        <v>2.5177144580129656</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C70" s="5">
+        <v>283.76349357015391</v>
+      </c>
+      <c r="D70" s="5">
+        <v>252.90325884297437</v>
+      </c>
+      <c r="E70" s="5">
+        <v>536.66675241312828</v>
+      </c>
+      <c r="F70" s="2">
+        <v>330.71333333333331</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0.52098615561042771</v>
+      </c>
+      <c r="H70" s="1">
+        <v>3.6344693554527061</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C71" s="5">
+        <v>401.86883136965241</v>
+      </c>
+      <c r="D71" s="5">
+        <v>516.52294029488996</v>
+      </c>
+      <c r="E71" s="5">
+        <v>918.39177166454238</v>
+      </c>
+      <c r="F71" s="2">
+        <v>375.83500000000004</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0.43169414651718552</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1.5039281705948373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C72" s="5">
+        <v>519.5798250216136</v>
+      </c>
+      <c r="D72" s="5">
+        <v>573.69377931549116</v>
+      </c>
+      <c r="E72" s="5">
+        <v>1093.2736043371046</v>
+      </c>
+      <c r="F72" s="2">
+        <v>386.05666666666662</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0.47497600643290355</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0.6228534298709737</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C73" s="5">
+        <v>409.14921969871932</v>
+      </c>
+      <c r="D73" s="5">
+        <v>433.38751789863011</v>
+      </c>
+      <c r="E73" s="5">
+        <v>842.53673759734943</v>
+      </c>
+      <c r="F73" s="2">
+        <v>366.61999999999995</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0.47372591273925724</v>
+      </c>
+      <c r="H73" s="1">
+        <v>2.3476570213412313</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C74" s="5">
+        <v>61.782113821138218</v>
+      </c>
+      <c r="D74" s="5">
+        <v>247.00787790053593</v>
+      </c>
+      <c r="E74" s="5">
+        <v>308.78999172167414</v>
+      </c>
+      <c r="F74" s="2">
+        <v>246.6</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0.202173563879401</v>
+      </c>
+      <c r="H74" s="1">
+        <v>3.5019110019110022</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C75" s="5">
+        <v>451.03560975609759</v>
+      </c>
+      <c r="D75" s="5">
+        <v>636.99580794609585</v>
+      </c>
+      <c r="E75" s="5">
+        <v>1088.0314177021935</v>
+      </c>
+      <c r="F75" s="2">
+        <v>297.20999999999998</v>
+      </c>
+      <c r="G75" s="6">
+        <v>0.41455245863152546</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.83741036991017592</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C76" s="5">
+        <v>350.88780487804871</v>
+      </c>
+      <c r="D76" s="5">
+        <v>624.32709224610971</v>
+      </c>
+      <c r="E76" s="5">
+        <v>975.21489712415837</v>
+      </c>
+      <c r="F76" s="2">
+        <v>303.27666666666664</v>
+      </c>
+      <c r="G76" s="6">
+        <v>0.35375306818484104</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1.0964912280701753</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C77" s="5">
+        <v>353.90691056910566</v>
+      </c>
+      <c r="D77" s="5">
+        <v>606.56594833635177</v>
+      </c>
+      <c r="E77" s="5">
+        <v>960.47285890545743</v>
+      </c>
+      <c r="F77" s="2">
+        <v>287.60500000000002</v>
+      </c>
+      <c r="G77" s="6">
+        <v>0.37538415770338429</v>
+      </c>
+      <c r="H77" s="1">
+        <v>2.6534869662212337</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C78" s="5">
+        <v>623.3024390243902</v>
+      </c>
+      <c r="D78" s="5">
+        <v>848.47580659390906</v>
+      </c>
+      <c r="E78" s="5">
+        <v>1471.7782456182993</v>
+      </c>
+      <c r="F78" s="2">
+        <v>334.57285714285712</v>
+      </c>
+      <c r="G78" s="6">
+        <v>0.42374779391562772</v>
+      </c>
+      <c r="H78" s="1">
+        <v>2.4574192153589403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2005</v>
+      </c>
+      <c r="C79" s="5">
+        <v>522.50878048780476</v>
+      </c>
+      <c r="D79" s="5">
+        <v>744.28224055356179</v>
+      </c>
+      <c r="E79" s="5">
+        <v>1266.7910210413665</v>
+      </c>
+      <c r="F79" s="2">
+        <v>340.89857142857142</v>
+      </c>
+      <c r="G79" s="6">
+        <v>0.40718744367780907</v>
+      </c>
+      <c r="H79" s="1">
+        <v>4.640211191760697</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C80" s="5">
+        <v>67.639535530173589</v>
+      </c>
+      <c r="D80" s="5">
+        <v>365.10039310905745</v>
+      </c>
+      <c r="E80" s="5">
+        <v>432.73992863923104</v>
+      </c>
+      <c r="F80" s="2">
+        <v>276.54000000000002</v>
+      </c>
+      <c r="G80" s="6">
+        <v>0.19514660147301455</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0.99663869496744473</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C81" s="5">
+        <v>381.24476555316983</v>
+      </c>
+      <c r="D81" s="5">
+        <v>403.8060898029575</v>
+      </c>
+      <c r="E81" s="5">
+        <v>785.05085535612739</v>
+      </c>
+      <c r="F81" s="2">
+        <v>338.8533333333333</v>
+      </c>
+      <c r="G81" s="6">
+        <v>0.51820903700124543</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0.59045570008321302</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C82" s="5">
+        <v>489.86381687632939</v>
+      </c>
+      <c r="D82" s="5">
+        <v>618.77299249937289</v>
+      </c>
+      <c r="E82" s="5">
+        <v>1108.6368093757023</v>
+      </c>
+      <c r="F82" s="2">
+        <v>368.39000000000004</v>
+      </c>
+      <c r="G82" s="6">
+        <v>0.44511510282066552</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1.3078395330724735</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C83" s="5">
+        <v>374.3991306064857</v>
+      </c>
+      <c r="D83" s="5">
+        <v>508.74399572247285</v>
+      </c>
+      <c r="E83" s="5">
+        <v>883.14312632895849</v>
+      </c>
+      <c r="F83" s="2">
+        <v>361.98666666666668</v>
+      </c>
+      <c r="G83" s="6">
+        <v>0.41726762669087658</v>
+      </c>
+      <c r="H83" s="1">
+        <v>3.1720933724576708</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C84" s="5">
+        <v>548.70987925806958</v>
+      </c>
+      <c r="D84" s="5">
+        <v>481.16614689565677</v>
+      </c>
+      <c r="E84" s="5">
+        <v>1029.8760261537263</v>
+      </c>
+      <c r="F84" s="2">
+        <v>377.42285714285714</v>
+      </c>
+      <c r="G84" s="6">
+        <v>0.5514880550125757</v>
+      </c>
+      <c r="H84" s="1">
+        <v>1.4356510784795695</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C85" s="5">
+        <v>570.74636885532072</v>
+      </c>
+      <c r="D85" s="5">
+        <v>445.42111583817297</v>
+      </c>
+      <c r="E85" s="5">
+        <v>1016.1674846934936</v>
+      </c>
+      <c r="F85" s="2">
+        <v>402.71857142857141</v>
+      </c>
+      <c r="G85" s="6">
+        <v>0.55953110436912268</v>
+      </c>
+      <c r="H85" s="1">
+        <v>1.0490396751553857</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
getting N response going
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="51">
   <si>
     <t>Year</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>AnnualFoliageHarvest</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>Cinput</t>
@@ -166,13 +163,19 @@
     <t>MakokaN24MaizeGliricidia</t>
   </si>
   <si>
-    <t>Thouseed</t>
-  </si>
-  <si>
     <t>HI</t>
   </si>
   <si>
     <t>%standloss</t>
+  </si>
+  <si>
+    <t>Clock.Today</t>
+  </si>
+  <si>
+    <t>Maize.Grain.Size</t>
+  </si>
+  <si>
+    <t>Maize.Grain.NumberFunction.Value</t>
   </si>
 </sst>
 </file>
@@ -1035,11 +1038,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241752208"/>
-        <c:axId val="241752600"/>
+        <c:axId val="405282856"/>
+        <c:axId val="405424624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241752208"/>
+        <c:axId val="405282856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,12 +1099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241752600"/>
+        <c:crossAx val="405424624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241752600"/>
+        <c:axId val="405424624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,7 +1161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241752208"/>
+        <c:crossAx val="405282856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1471,11 +1474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241753384"/>
-        <c:axId val="241753776"/>
+        <c:axId val="405363096"/>
+        <c:axId val="405363480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241753384"/>
+        <c:axId val="405363096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,12 +1535,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241753776"/>
+        <c:crossAx val="405363480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241753776"/>
+        <c:axId val="405363480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,7 +1597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241753384"/>
+        <c:crossAx val="405363096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1905,11 +1908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241754560"/>
-        <c:axId val="241754952"/>
+        <c:axId val="406223832"/>
+        <c:axId val="406352680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241754560"/>
+        <c:axId val="406223832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,12 +1969,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241754952"/>
+        <c:crossAx val="406352680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241754952"/>
+        <c:axId val="406352680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241754560"/>
+        <c:crossAx val="406223832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4121,18 +4124,18 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>34991</v>
@@ -4144,7 +4147,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4">
         <v>35049</v>
@@ -4159,7 +4162,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4">
         <v>35082</v>
@@ -4174,7 +4177,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4">
         <v>35118</v>
@@ -4189,7 +4192,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4">
         <v>35139</v>
@@ -4204,7 +4207,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4">
         <v>35174</v>
@@ -4219,7 +4222,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>35244</v>
@@ -4234,7 +4237,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4">
         <v>35307</v>
@@ -4249,7 +4252,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4">
         <v>35377</v>
@@ -4264,7 +4267,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4">
         <v>35409</v>
@@ -4279,7 +4282,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>35074</v>
@@ -4294,7 +4297,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4">
         <v>35460</v>
@@ -4305,7 +4308,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>35489</v>
@@ -4320,7 +4323,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="4">
         <v>35548</v>
@@ -4335,7 +4338,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4">
         <v>35649</v>
@@ -4350,7 +4353,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="4">
         <v>35754</v>
@@ -4362,7 +4365,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4">
         <v>34991</v>
@@ -4374,7 +4377,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4">
         <v>35049</v>
@@ -4388,7 +4391,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4">
         <v>35082</v>
@@ -4402,7 +4405,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4">
         <v>35118</v>
@@ -4416,7 +4419,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="4">
         <v>35139</v>
@@ -4430,7 +4433,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4">
         <v>35174</v>
@@ -4444,7 +4447,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4">
         <v>35244</v>
@@ -4458,7 +4461,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="4">
         <v>35307</v>
@@ -4472,7 +4475,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4">
         <v>35377</v>
@@ -4486,7 +4489,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4">
         <v>35409</v>
@@ -4500,7 +4503,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4">
         <v>35074</v>
@@ -4514,7 +4517,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="4">
         <v>35460</v>
@@ -4525,7 +4528,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="4">
         <v>35489</v>
@@ -4539,7 +4542,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="4">
         <v>35548</v>
@@ -4553,7 +4556,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="4">
         <v>35649</v>
@@ -4567,7 +4570,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4">
         <v>35754</v>
@@ -4579,7 +4582,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4">
         <v>34991</v>
@@ -4591,7 +4594,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="4">
         <v>35049</v>
@@ -4605,7 +4608,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4">
         <v>35082</v>
@@ -4619,7 +4622,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="4">
         <v>35118</v>
@@ -4633,7 +4636,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="4">
         <v>35139</v>
@@ -4647,7 +4650,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="4">
         <v>35174</v>
@@ -4661,7 +4664,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="4">
         <v>35244</v>
@@ -4675,7 +4678,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4">
         <v>35307</v>
@@ -4689,7 +4692,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="4">
         <v>35377</v>
@@ -4703,7 +4706,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4">
         <v>35409</v>
@@ -4717,7 +4720,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4">
         <v>35074</v>
@@ -4731,7 +4734,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="4">
         <v>35460</v>
@@ -4742,7 +4745,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="4">
         <v>35489</v>
@@ -4756,7 +4759,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="4">
         <v>35548</v>
@@ -4770,7 +4773,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="4">
         <v>35649</v>
@@ -4784,7 +4787,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="4">
         <v>35754</v>
@@ -4795,7 +4798,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="4">
         <v>34991</v>
@@ -4806,7 +4809,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="4">
         <v>35049</v>
@@ -4820,7 +4823,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="4">
         <v>35082</v>
@@ -4834,7 +4837,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="4">
         <v>35118</v>
@@ -4848,7 +4851,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="4">
         <v>35139</v>
@@ -4862,7 +4865,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" s="4">
         <v>35174</v>
@@ -4876,7 +4879,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B56" s="4">
         <v>35244</v>
@@ -4890,7 +4893,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57" s="4">
         <v>35307</v>
@@ -4904,7 +4907,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B58" s="4">
         <v>35377</v>
@@ -4918,7 +4921,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="4">
         <v>35409</v>
@@ -4932,7 +4935,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" s="4">
         <v>35074</v>
@@ -4946,7 +4949,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B61" s="4">
         <v>35460</v>
@@ -4957,7 +4960,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="4">
         <v>35489</v>
@@ -4971,7 +4974,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B63" s="4">
         <v>35548</v>
@@ -4985,7 +4988,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B64" s="4">
         <v>35649</v>
@@ -4999,7 +5002,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B65" s="4">
         <v>35754</v>
@@ -5018,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5037,7 +5040,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -5046,31 +5049,31 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>34</v>
-      </c>
       <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -5355,7 +5358,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <f>YEAR(C13)</f>
@@ -5381,7 +5384,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B28" si="3">YEAR(C14)</f>
@@ -5407,7 +5410,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <f t="shared" si="3"/>
@@ -5433,7 +5436,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <f t="shared" si="3"/>
@@ -5459,7 +5462,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <f t="shared" si="3"/>
@@ -5485,7 +5488,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <f t="shared" si="3"/>
@@ -5511,7 +5514,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <f t="shared" si="3"/>
@@ -5537,7 +5540,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <f t="shared" si="3"/>
@@ -5563,7 +5566,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <f t="shared" si="3"/>
@@ -5589,7 +5592,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <f t="shared" si="3"/>
@@ -5615,7 +5618,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <f t="shared" si="3"/>
@@ -5641,7 +5644,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <f t="shared" si="3"/>
@@ -5667,7 +5670,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <f t="shared" si="3"/>
@@ -5693,7 +5696,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <f t="shared" si="3"/>
@@ -5719,7 +5722,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <f t="shared" si="3"/>
@@ -5733,7 +5736,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <f t="shared" si="3"/>
@@ -5747,7 +5750,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3">
         <v>35184</v>
@@ -5770,7 +5773,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3">
         <v>35236</v>
@@ -5793,7 +5796,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3">
         <v>35290</v>
@@ -5816,7 +5819,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="3">
         <v>35348</v>
@@ -5839,7 +5842,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="3">
         <v>35400</v>
@@ -5862,7 +5865,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="3">
         <v>35461</v>
@@ -5885,7 +5888,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3">
         <v>35184</v>
@@ -5908,7 +5911,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="3">
         <v>35236</v>
@@ -5931,7 +5934,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="3">
         <v>35289</v>
@@ -5954,7 +5957,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3">
         <v>35290</v>
@@ -5974,7 +5977,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="3">
         <v>35348</v>
@@ -5997,7 +6000,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="3">
         <v>35400</v>
@@ -6020,7 +6023,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="3">
         <v>35461</v>
@@ -6043,7 +6046,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="3">
         <v>35184</v>
@@ -6066,7 +6069,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="3">
         <v>35245</v>
@@ -6089,7 +6092,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44" s="3">
         <v>35236</v>
@@ -6109,7 +6112,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="3">
         <v>35290</v>
@@ -6132,7 +6135,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" s="3">
         <v>35291</v>
@@ -6150,7 +6153,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="3">
         <v>35347</v>
@@ -6171,7 +6174,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" s="3">
         <v>35348</v>
@@ -6189,7 +6192,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C49" s="3">
         <v>35399</v>
@@ -6210,7 +6213,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50" s="3">
         <v>35400</v>
@@ -6231,7 +6234,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C51" s="3">
         <v>35461</v>
@@ -6338,18 +6341,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -6357,27 +6361,30 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2">
         <v>1993</v>
@@ -6391,13 +6398,13 @@
       <c r="E2" s="5">
         <v>449.4</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>0.44370271473075212</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
         <v>1993</v>
@@ -6407,11 +6414,11 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
         <v>1993</v>
@@ -6421,11 +6428,11 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2">
         <v>1993</v>
@@ -6439,13 +6446,13 @@
       <c r="E5" s="5">
         <v>340.7</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>0.48635162899911943</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <v>1993</v>
@@ -6455,11 +6462,11 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2">
         <v>1993</v>
@@ -6469,11 +6476,11 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2">
         <v>1994</v>
@@ -6487,13 +6494,13 @@
       <c r="E8" s="5">
         <v>325.10000000000002</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>0.46170409104890797</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2">
         <v>1994</v>
@@ -6503,11 +6510,11 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2">
         <v>1994</v>
@@ -6517,11 +6524,11 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2">
         <v>1994</v>
@@ -6535,13 +6542,13 @@
       <c r="E11" s="5">
         <v>817.2</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>0.47993147332354374</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2">
         <v>1994</v>
@@ -6551,11 +6558,11 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2">
         <v>1994</v>
@@ -6565,11 +6572,11 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2">
         <v>1995</v>
@@ -6583,13 +6590,13 @@
       <c r="E14" s="5">
         <v>324</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>0.45987654320987653</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2">
         <v>1995</v>
@@ -6599,11 +6606,11 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2">
         <v>1995</v>
@@ -6613,11 +6620,11 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2">
         <v>1995</v>
@@ -6631,13 +6638,13 @@
       <c r="E17" s="5">
         <v>623.4</v>
       </c>
-      <c r="G17" s="6">
+      <c r="H17" s="6">
         <v>0.47866538338145653</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2">
         <v>1995</v>
@@ -6647,11 +6654,11 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2">
         <v>1995</v>
@@ -6661,11 +6668,11 @@
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
         <v>1996</v>
@@ -6679,13 +6686,13 @@
       <c r="E20" s="5">
         <v>270</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>1996</v>
@@ -6695,11 +6702,11 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2">
         <v>1996</v>
@@ -6709,11 +6716,11 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2">
         <v>1996</v>
@@ -6727,13 +6734,13 @@
       <c r="E23" s="5">
         <v>1130.2</v>
       </c>
-      <c r="G23" s="6">
+      <c r="H23" s="6">
         <v>0.46912050964431079</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2">
         <v>1996</v>
@@ -6743,11 +6750,11 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2">
         <v>1996</v>
@@ -6757,11 +6764,11 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2">
         <v>1997</v>
@@ -6775,13 +6782,13 @@
       <c r="E26" s="5">
         <v>127.9</v>
       </c>
-      <c r="G26" s="6">
+      <c r="H26" s="6">
         <v>0.41360437842064107</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2">
         <v>1997</v>
@@ -6791,11 +6798,11 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2">
         <v>1997</v>
@@ -6805,11 +6812,11 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
         <v>1997</v>
@@ -6823,13 +6830,13 @@
       <c r="E29" s="5">
         <v>710.6</v>
       </c>
-      <c r="G29" s="6">
+      <c r="H29" s="6">
         <v>0.47227694905713485</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2">
         <v>1997</v>
@@ -6839,11 +6846,11 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2">
         <v>1997</v>
@@ -6853,11 +6860,11 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2">
         <v>1998</v>
@@ -6871,13 +6878,13 @@
       <c r="E32" s="5">
         <v>232.3</v>
       </c>
-      <c r="G32" s="6">
+      <c r="H32" s="6">
         <v>0.46190271201033145</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2">
         <v>1998</v>
@@ -6887,11 +6894,11 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2">
         <v>1998</v>
@@ -6901,11 +6908,11 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2">
         <v>1998</v>
@@ -6919,13 +6926,13 @@
       <c r="E35" s="5">
         <v>907.2</v>
       </c>
-      <c r="G35" s="6">
+      <c r="H35" s="6">
         <v>0.47641093474426804</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="2">
         <v>1998</v>
@@ -6935,11 +6942,11 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2">
         <v>1998</v>
@@ -6949,11 +6956,11 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2">
         <v>1999</v>
@@ -6968,14 +6975,15 @@
         <v>226.5</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="6">
+      <c r="G38" s="2"/>
+      <c r="H38" s="6">
         <v>0.44812362030905079</v>
       </c>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2">
         <v>1999</v>
@@ -6986,12 +6994,13 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G39" s="2"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2">
         <v>1999</v>
@@ -7002,12 +7011,13 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G40" s="2"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2">
         <v>1999</v>
@@ -7022,14 +7032,15 @@
         <v>948.7</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="6">
+      <c r="G41" s="2"/>
+      <c r="H41" s="6">
         <v>0.47296300200274055</v>
       </c>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="2">
         <v>1999</v>
@@ -7040,12 +7051,13 @@
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G42" s="2"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2">
         <v>1999</v>
@@ -7056,12 +7068,13 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G43" s="2"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="2">
         <v>2000</v>
@@ -7076,14 +7089,15 @@
         <v>180.4</v>
       </c>
       <c r="F44" s="2"/>
-      <c r="G44" s="6">
+      <c r="G44" s="2"/>
+      <c r="H44" s="6">
         <v>0.44567627494456763</v>
       </c>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2">
         <v>2000</v>
@@ -7094,12 +7108,13 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G45" s="2"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" s="2">
         <v>2000</v>
@@ -7110,12 +7125,13 @@
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G46" s="2"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="2">
         <v>2000</v>
@@ -7130,14 +7146,15 @@
         <v>505.9</v>
       </c>
       <c r="F47" s="2"/>
-      <c r="G47" s="6">
+      <c r="G47" s="2"/>
+      <c r="H47" s="6">
         <v>0.45641431112868158</v>
       </c>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2">
         <v>2000</v>
@@ -7148,12 +7165,13 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G48" s="2"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2">
         <v>2000</v>
@@ -7164,12 +7182,13 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G49" s="2"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2">
         <v>2001</v>
@@ -7184,14 +7203,15 @@
         <v>185.7</v>
       </c>
       <c r="F50" s="2"/>
-      <c r="G50" s="6">
+      <c r="G50" s="2"/>
+      <c r="H50" s="6">
         <v>0.46149703823371035</v>
       </c>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="2">
         <v>2001</v>
@@ -7202,12 +7222,13 @@
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G51" s="2"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B52" s="2">
         <v>2001</v>
@@ -7218,12 +7239,13 @@
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G52" s="2"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2">
         <v>2001</v>
@@ -7238,14 +7260,15 @@
         <v>1080.9000000000001</v>
       </c>
       <c r="F53" s="2"/>
-      <c r="G53" s="6">
+      <c r="G53" s="2"/>
+      <c r="H53" s="6">
         <v>0.46803589601258205</v>
       </c>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B54" s="2">
         <v>2001</v>
@@ -7256,12 +7279,13 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G54" s="2"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" s="2">
         <v>2001</v>
@@ -7272,12 +7296,13 @@
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G55" s="2"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" s="2">
         <v>2002</v>
@@ -7292,14 +7317,15 @@
         <v>200</v>
       </c>
       <c r="F56" s="2"/>
-      <c r="G56" s="6">
+      <c r="G56" s="2"/>
+      <c r="H56" s="6">
         <v>0.5</v>
       </c>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B57" s="2">
         <v>2002</v>
@@ -7310,12 +7336,13 @@
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G57" s="2"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="2">
         <v>2002</v>
@@ -7326,12 +7353,13 @@
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G58" s="2"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B59" s="2">
         <v>2002</v>
@@ -7346,14 +7374,15 @@
         <v>890</v>
       </c>
       <c r="F59" s="2"/>
-      <c r="G59" s="6">
+      <c r="G59" s="2"/>
+      <c r="H59" s="6">
         <v>0.46629213483146065</v>
       </c>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2">
         <v>2002</v>
@@ -7364,12 +7393,13 @@
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G60" s="2"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B61" s="2">
         <v>2002</v>
@@ -7380,12 +7410,13 @@
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G61" s="2"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B62" s="2">
         <v>2003</v>
@@ -7399,19 +7430,23 @@
       <c r="E62" s="5">
         <v>303.29667823366469</v>
       </c>
-      <c r="F62" s="2">
-        <v>311.11666666666662</v>
+      <c r="F62" s="6">
+        <v>0.3111166666666666</v>
       </c>
       <c r="G62" s="6">
+        <f>C62/F62</f>
+        <v>474.86225202424527</v>
+      </c>
+      <c r="H62" s="6">
         <v>0.48834578500969578</v>
       </c>
-      <c r="H62" s="1">
+      <c r="I62" s="1">
         <v>20.174684645498044</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="2">
         <v>2003</v>
@@ -7425,19 +7460,23 @@
       <c r="E63" s="5">
         <v>695.40248857655354</v>
       </c>
-      <c r="F63" s="2">
-        <v>377.26333333333332</v>
+      <c r="F63" s="6">
+        <v>0.37726333333333334</v>
       </c>
       <c r="G63" s="6">
+        <f t="shared" ref="G63:G85" si="0">C63/F63</f>
+        <v>862.90570581157976</v>
+      </c>
+      <c r="H63" s="6">
         <v>0.46296529638549005</v>
       </c>
-      <c r="H63" s="1">
+      <c r="I63" s="1">
         <v>12.614615807812214</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B64" s="2">
         <v>2003</v>
@@ -7451,19 +7490,23 @@
       <c r="E64" s="5">
         <v>583.68871520588868</v>
       </c>
-      <c r="F64" s="2">
-        <v>330.28</v>
+      <c r="F64" s="6">
+        <v>0.33027999999999996</v>
       </c>
       <c r="G64" s="6">
+        <f t="shared" si="0"/>
+        <v>874.01869416538432</v>
+      </c>
+      <c r="H64" s="6">
         <v>0.49304866218202514</v>
       </c>
-      <c r="H64" s="1">
+      <c r="I64" s="1">
         <v>10.2986955631914</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" s="2">
         <v>2003</v>
@@ -7477,19 +7520,23 @@
       <c r="E65" s="5">
         <v>974.36807525844506</v>
       </c>
-      <c r="F65" s="2">
-        <v>412.77500000000003</v>
+      <c r="F65" s="6">
+        <v>0.41277500000000006</v>
       </c>
       <c r="G65" s="6">
+        <f t="shared" si="0"/>
+        <v>1190.682850999063</v>
+      </c>
+      <c r="H65" s="6">
         <v>0.50308413969094035</v>
       </c>
-      <c r="H65" s="1">
+      <c r="I65" s="1">
         <v>17.604570573283841</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" s="2">
         <v>2003</v>
@@ -7503,19 +7550,23 @@
       <c r="E66" s="5">
         <v>1143.027788883029</v>
       </c>
-      <c r="F66" s="2">
-        <v>418.03</v>
+      <c r="F66" s="6">
+        <v>0.41802999999999996</v>
       </c>
       <c r="G66" s="6">
+        <f t="shared" si="0"/>
+        <v>1355.1197068557535</v>
+      </c>
+      <c r="H66" s="6">
         <v>0.49478288809734661</v>
       </c>
-      <c r="H66" s="1">
+      <c r="I66" s="1">
         <v>15.271238981895833</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B67" s="2">
         <v>2003</v>
@@ -7529,19 +7580,23 @@
       <c r="E67" s="5">
         <v>1068.1286610612151</v>
       </c>
-      <c r="F67" s="2">
-        <v>388.0116666666666</v>
+      <c r="F67" s="6">
+        <v>0.38801166666666659</v>
       </c>
       <c r="G67" s="6">
+        <f t="shared" si="0"/>
+        <v>1290.7075650541481</v>
+      </c>
+      <c r="H67" s="6">
         <v>0.47731697382290128</v>
       </c>
-      <c r="H67" s="1">
+      <c r="I67" s="1">
         <v>16.095937452239973</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="2">
         <v>2004</v>
@@ -7555,19 +7610,23 @@
       <c r="E68" s="5">
         <v>275.45979119495979</v>
       </c>
-      <c r="F68" s="2">
-        <v>297.19666666666666</v>
+      <c r="F68" s="6">
+        <v>0.29719666666666666</v>
       </c>
       <c r="G68" s="6">
+        <f t="shared" si="0"/>
+        <v>366.94876554807718</v>
+      </c>
+      <c r="H68" s="6">
         <v>0.39853687851550257</v>
       </c>
-      <c r="H68" s="1">
+      <c r="I68" s="1">
         <v>2.035973976272484</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B69" s="2">
         <v>2004</v>
@@ -7581,19 +7640,23 @@
       <c r="E69" s="5">
         <v>626.24520573897598</v>
       </c>
-      <c r="F69" s="2">
-        <v>348.52333333333331</v>
+      <c r="F69" s="6">
+        <v>0.3485233333333333</v>
       </c>
       <c r="G69" s="6">
+        <f t="shared" si="0"/>
+        <v>914.60877337923398</v>
+      </c>
+      <c r="H69" s="6">
         <v>0.50808374593232708</v>
       </c>
-      <c r="H69" s="1">
+      <c r="I69" s="1">
         <v>2.5177144580129656</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" s="2">
         <v>2004</v>
@@ -7607,19 +7670,23 @@
       <c r="E70" s="5">
         <v>536.66675241312828</v>
       </c>
-      <c r="F70" s="2">
-        <v>330.71333333333331</v>
+      <c r="F70" s="6">
+        <v>0.3307133333333333</v>
       </c>
       <c r="G70" s="6">
+        <f t="shared" si="0"/>
+        <v>858.0346329252543</v>
+      </c>
+      <c r="H70" s="6">
         <v>0.52098615561042771</v>
       </c>
-      <c r="H70" s="1">
+      <c r="I70" s="1">
         <v>3.6344693554527061</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71" s="2">
         <v>2004</v>
@@ -7633,19 +7700,23 @@
       <c r="E71" s="5">
         <v>918.39177166454238</v>
       </c>
-      <c r="F71" s="2">
-        <v>375.83500000000004</v>
+      <c r="F71" s="6">
+        <v>0.37583500000000003</v>
       </c>
       <c r="G71" s="6">
+        <f t="shared" si="0"/>
+        <v>1069.2693106540166</v>
+      </c>
+      <c r="H71" s="6">
         <v>0.43169414651718552</v>
       </c>
-      <c r="H71" s="1">
+      <c r="I71" s="1">
         <v>1.5039281705948373</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B72" s="2">
         <v>2004</v>
@@ -7659,19 +7730,23 @@
       <c r="E72" s="5">
         <v>1093.2736043371046</v>
       </c>
-      <c r="F72" s="2">
-        <v>386.05666666666662</v>
+      <c r="F72" s="6">
+        <v>0.3860566666666666</v>
       </c>
       <c r="G72" s="6">
+        <f t="shared" si="0"/>
+        <v>1345.8641434891606</v>
+      </c>
+      <c r="H72" s="6">
         <v>0.47497600643290355</v>
       </c>
-      <c r="H72" s="1">
+      <c r="I72" s="1">
         <v>0.6228534298709737</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B73" s="2">
         <v>2004</v>
@@ -7685,19 +7760,23 @@
       <c r="E73" s="5">
         <v>842.53673759734943</v>
       </c>
-      <c r="F73" s="2">
-        <v>366.61999999999995</v>
+      <c r="F73" s="6">
+        <v>0.36661999999999995</v>
       </c>
       <c r="G73" s="6">
+        <f t="shared" si="0"/>
+        <v>1116.0035450840635</v>
+      </c>
+      <c r="H73" s="6">
         <v>0.47372591273925724</v>
       </c>
-      <c r="H73" s="1">
+      <c r="I73" s="1">
         <v>2.3476570213412313</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B74" s="2">
         <v>2005</v>
@@ -7711,19 +7790,23 @@
       <c r="E74" s="5">
         <v>308.78999172167414</v>
       </c>
-      <c r="F74" s="2">
-        <v>246.6</v>
+      <c r="F74" s="6">
+        <v>0.24659999999999999</v>
       </c>
       <c r="G74" s="6">
+        <f t="shared" si="0"/>
+        <v>250.53574136714607</v>
+      </c>
+      <c r="H74" s="6">
         <v>0.202173563879401</v>
       </c>
-      <c r="H74" s="1">
+      <c r="I74" s="1">
         <v>3.5019110019110022</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B75" s="2">
         <v>2005</v>
@@ -7737,19 +7820,23 @@
       <c r="E75" s="5">
         <v>1088.0314177021935</v>
       </c>
-      <c r="F75" s="2">
-        <v>297.20999999999998</v>
+      <c r="F75" s="6">
+        <v>0.29720999999999997</v>
       </c>
       <c r="G75" s="6">
+        <f t="shared" si="0"/>
+        <v>1517.5653906534021</v>
+      </c>
+      <c r="H75" s="6">
         <v>0.41455245863152546</v>
       </c>
-      <c r="H75" s="1">
+      <c r="I75" s="1">
         <v>0.83741036991017592</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="2">
         <v>2005</v>
@@ -7763,19 +7850,23 @@
       <c r="E76" s="5">
         <v>975.21489712415837</v>
       </c>
-      <c r="F76" s="2">
-        <v>303.27666666666664</v>
+      <c r="F76" s="6">
+        <v>0.30327666666666664</v>
       </c>
       <c r="G76" s="6">
+        <f t="shared" si="0"/>
+        <v>1156.9891239397978</v>
+      </c>
+      <c r="H76" s="6">
         <v>0.35375306818484104</v>
       </c>
-      <c r="H76" s="1">
+      <c r="I76" s="1">
         <v>1.0964912280701753</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B77" s="2">
         <v>2005</v>
@@ -7789,19 +7880,23 @@
       <c r="E77" s="5">
         <v>960.47285890545743</v>
       </c>
-      <c r="F77" s="2">
-        <v>287.60500000000002</v>
+      <c r="F77" s="6">
+        <v>0.287605</v>
       </c>
       <c r="G77" s="6">
+        <f t="shared" si="0"/>
+        <v>1230.5311471257651</v>
+      </c>
+      <c r="H77" s="6">
         <v>0.37538415770338429</v>
       </c>
-      <c r="H77" s="1">
+      <c r="I77" s="1">
         <v>2.6534869662212337</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B78" s="2">
         <v>2005</v>
@@ -7815,19 +7910,23 @@
       <c r="E78" s="5">
         <v>1471.7782456182993</v>
       </c>
-      <c r="F78" s="2">
-        <v>334.57285714285712</v>
+      <c r="F78" s="6">
+        <v>0.33457285714285712</v>
       </c>
       <c r="G78" s="6">
+        <f t="shared" si="0"/>
+        <v>1862.9796940110127</v>
+      </c>
+      <c r="H78" s="6">
         <v>0.42374779391562772</v>
       </c>
-      <c r="H78" s="1">
+      <c r="I78" s="1">
         <v>2.4574192153589403</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" s="2">
         <v>2005</v>
@@ -7841,19 +7940,23 @@
       <c r="E79" s="5">
         <v>1266.7910210413665</v>
       </c>
-      <c r="F79" s="2">
-        <v>340.89857142857142</v>
+      <c r="F79" s="6">
+        <v>0.34089857142857144</v>
       </c>
       <c r="G79" s="6">
+        <f t="shared" si="0"/>
+        <v>1532.739718732691</v>
+      </c>
+      <c r="H79" s="6">
         <v>0.40718744367780907</v>
       </c>
-      <c r="H79" s="1">
+      <c r="I79" s="1">
         <v>4.640211191760697</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B80" s="2">
         <v>2006</v>
@@ -7867,19 +7970,23 @@
       <c r="E80" s="5">
         <v>432.73992863923104</v>
       </c>
-      <c r="F80" s="2">
-        <v>276.54000000000002</v>
+      <c r="F80" s="6">
+        <v>0.27654000000000001</v>
       </c>
       <c r="G80" s="6">
+        <f t="shared" si="0"/>
+        <v>244.5922308894684</v>
+      </c>
+      <c r="H80" s="6">
         <v>0.19514660147301455</v>
       </c>
-      <c r="H80" s="1">
+      <c r="I80" s="1">
         <v>0.99663869496744473</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B81" s="2">
         <v>2006</v>
@@ -7893,19 +8000,23 @@
       <c r="E81" s="5">
         <v>785.05085535612739</v>
       </c>
-      <c r="F81" s="2">
-        <v>338.8533333333333</v>
+      <c r="F81" s="6">
+        <v>0.33885333333333328</v>
       </c>
       <c r="G81" s="6">
+        <f t="shared" si="0"/>
+        <v>1125.102597642549</v>
+      </c>
+      <c r="H81" s="6">
         <v>0.51820903700124543</v>
       </c>
-      <c r="H81" s="1">
+      <c r="I81" s="1">
         <v>0.59045570008321302</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="2">
         <v>2006</v>
@@ -7919,19 +8030,23 @@
       <c r="E82" s="5">
         <v>1108.6368093757023</v>
       </c>
-      <c r="F82" s="2">
-        <v>368.39000000000004</v>
+      <c r="F82" s="6">
+        <v>0.36839000000000005</v>
       </c>
       <c r="G82" s="6">
+        <f t="shared" si="0"/>
+        <v>1329.7424383841292</v>
+      </c>
+      <c r="H82" s="6">
         <v>0.44511510282066552</v>
       </c>
-      <c r="H82" s="1">
+      <c r="I82" s="1">
         <v>1.3078395330724735</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="2">
         <v>2006</v>
@@ -7945,19 +8060,23 @@
       <c r="E83" s="5">
         <v>883.14312632895849</v>
       </c>
-      <c r="F83" s="2">
-        <v>361.98666666666668</v>
+      <c r="F83" s="6">
+        <v>0.36198666666666668</v>
       </c>
       <c r="G83" s="6">
+        <f t="shared" si="0"/>
+        <v>1034.289837396826</v>
+      </c>
+      <c r="H83" s="6">
         <v>0.41726762669087658</v>
       </c>
-      <c r="H83" s="1">
+      <c r="I83" s="1">
         <v>3.1720933724576708</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B84" s="2">
         <v>2006</v>
@@ -7971,19 +8090,23 @@
       <c r="E84" s="5">
         <v>1029.8760261537263</v>
       </c>
-      <c r="F84" s="2">
-        <v>377.42285714285714</v>
+      <c r="F84" s="6">
+        <v>0.37742285714285712</v>
       </c>
       <c r="G84" s="6">
+        <f t="shared" si="0"/>
+        <v>1453.8331976284605</v>
+      </c>
+      <c r="H84" s="6">
         <v>0.5514880550125757</v>
       </c>
-      <c r="H84" s="1">
+      <c r="I84" s="1">
         <v>1.4356510784795695</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B85" s="2">
         <v>2006</v>
@@ -7997,13 +8120,17 @@
       <c r="E85" s="5">
         <v>1016.1674846934936</v>
       </c>
-      <c r="F85" s="2">
-        <v>402.71857142857141</v>
+      <c r="F85" s="6">
+        <v>0.40271857142857143</v>
       </c>
       <c r="G85" s="6">
+        <f t="shared" si="0"/>
+        <v>1417.2337938891196</v>
+      </c>
+      <c r="H85" s="6">
         <v>0.55953110436912268</v>
       </c>
-      <c r="H85" s="1">
+      <c r="I85" s="1">
         <v>1.0490396751553857</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Makoka cutting schedule to match observed
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -1076,11 +1076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223097472"/>
-        <c:axId val="223097864"/>
+        <c:axId val="225712384"/>
+        <c:axId val="225712768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223097472"/>
+        <c:axId val="225712384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,12 +1137,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223097864"/>
+        <c:crossAx val="225712768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223097864"/>
+        <c:axId val="225712768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223097472"/>
+        <c:crossAx val="225712384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1514,11 +1514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223098648"/>
-        <c:axId val="223099040"/>
+        <c:axId val="225415704"/>
+        <c:axId val="224755272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223098648"/>
+        <c:axId val="225415704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,12 +1575,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223099040"/>
+        <c:crossAx val="224755272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223099040"/>
+        <c:axId val="224755272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223098648"/>
+        <c:crossAx val="225415704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1949,11 +1949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223099824"/>
-        <c:axId val="223100216"/>
+        <c:axId val="225442288"/>
+        <c:axId val="225459192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223099824"/>
+        <c:axId val="225442288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,12 +2010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223100216"/>
+        <c:crossAx val="225459192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223100216"/>
+        <c:axId val="225459192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223099824"/>
+        <c:crossAx val="225442288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5062,10 +5062,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3168" topLeftCell="A78" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3168" topLeftCell="A66" activePane="bottomLeft"/>
       <selection activeCell="O2" sqref="O2"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101:A105"/>
+      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6321,6 +6321,10 @@
       <c r="C52" s="12">
         <v>33862</v>
       </c>
+      <c r="H52">
+        <f>M52+O52</f>
+        <v>178</v>
+      </c>
       <c r="M52" s="10">
         <v>152</v>
       </c>
@@ -6379,6 +6383,10 @@
       </c>
       <c r="C55" s="12">
         <v>34227</v>
+      </c>
+      <c r="H55">
+        <f>M55+O55</f>
+        <v>266</v>
       </c>
       <c r="M55" s="10">
         <v>243</v>
@@ -6453,6 +6461,10 @@
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
+      <c r="H58">
+        <f>M58+O58</f>
+        <v>216</v>
+      </c>
       <c r="J58" s="9"/>
       <c r="M58" s="10">
         <v>141</v>
@@ -6517,6 +6529,10 @@
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
+      <c r="H61">
+        <f>M61+O61</f>
+        <v>265</v>
+      </c>
       <c r="J61" s="9"/>
       <c r="M61" s="10">
         <v>136</v>
@@ -6567,6 +6583,10 @@
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
+      <c r="H64">
+        <f>M64+O64</f>
+        <v>309</v>
+      </c>
       <c r="J64" s="9"/>
       <c r="M64" s="10">
         <v>142</v>
@@ -6617,6 +6637,10 @@
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
+      <c r="H67">
+        <f>M67+O67</f>
+        <v>209</v>
+      </c>
       <c r="J67" s="9"/>
       <c r="M67" s="10">
         <v>209</v>
@@ -6683,6 +6707,10 @@
       <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
+      <c r="H71">
+        <f>M71+O71</f>
+        <v>335</v>
+      </c>
       <c r="J71" s="11"/>
       <c r="M71" s="10">
         <v>335</v>
@@ -6749,6 +6777,10 @@
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
+      <c r="H75">
+        <f>M75+O75</f>
+        <v>340</v>
+      </c>
       <c r="J75" s="11"/>
       <c r="M75" s="10">
         <v>340</v>
@@ -6815,6 +6847,10 @@
       <c r="E79" s="10"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
+      <c r="H79">
+        <f>M79+O79</f>
+        <v>451</v>
+      </c>
       <c r="J79" s="11"/>
       <c r="M79" s="10">
         <v>450</v>
@@ -6881,6 +6917,10 @@
       <c r="E83" s="10"/>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
+      <c r="H83">
+        <f>M83+O83</f>
+        <v>400</v>
+      </c>
       <c r="J83" s="11"/>
       <c r="M83" s="10">
         <v>400</v>
@@ -6947,6 +6987,10 @@
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
+      <c r="H87">
+        <f>M87+O87</f>
+        <v>400</v>
+      </c>
       <c r="J87" s="11"/>
       <c r="M87" s="10">
         <v>400</v>
@@ -7013,6 +7057,10 @@
       <c r="E91" s="10"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
+      <c r="H91">
+        <f>M91+O91</f>
+        <v>678</v>
+      </c>
       <c r="J91" s="11"/>
       <c r="M91" s="10">
         <v>320</v>
@@ -7079,6 +7127,10 @@
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
+      <c r="H95">
+        <f>M95+O95</f>
+        <v>264</v>
+      </c>
       <c r="J95" s="11"/>
       <c r="M95" s="10">
         <v>173</v>
@@ -7129,6 +7181,10 @@
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
+      <c r="H98">
+        <f>M98+O98</f>
+        <v>580</v>
+      </c>
       <c r="J98" s="9"/>
       <c r="M98" s="10">
         <v>401</v>

</xml_diff>

<commit_message>
New observed, met and soil data
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Gliricidia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SME016\Dropbox\AgroforestryModelDevelopment\Gliricidia Model\Gliricidia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9888" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedSoil" sheetId="12" r:id="rId1"/>
@@ -1076,11 +1076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225712384"/>
-        <c:axId val="225712768"/>
+        <c:axId val="417230912"/>
+        <c:axId val="418888656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225712384"/>
+        <c:axId val="417230912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,12 +1137,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225712768"/>
+        <c:crossAx val="418888656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225712768"/>
+        <c:axId val="418888656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225712384"/>
+        <c:crossAx val="417230912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1514,11 +1514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225415704"/>
-        <c:axId val="224755272"/>
+        <c:axId val="420240520"/>
+        <c:axId val="420241696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225415704"/>
+        <c:axId val="420240520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,12 +1575,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224755272"/>
+        <c:crossAx val="420241696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="224755272"/>
+        <c:axId val="420241696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225415704"/>
+        <c:crossAx val="420240520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1949,11 +1949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225442288"/>
-        <c:axId val="225459192"/>
+        <c:axId val="172053416"/>
+        <c:axId val="414785368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225442288"/>
+        <c:axId val="172053416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2010,12 +2010,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225459192"/>
+        <c:crossAx val="414785368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225459192"/>
+        <c:axId val="414785368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225442288"/>
+        <c:crossAx val="172053416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4153,14 +4153,14 @@
       <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -4276,7 +4276,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>9.0359999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>49.505000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>33.975000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>18.78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>23.655000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>16.782</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>36.835000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>49.939</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>42.816000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>27.969000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>116.55500000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>5.7110000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>19.163</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>41.692</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>33.709000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>39.747999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>13.172000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>23.315999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>17.97</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>38.872999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>19.538</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>33.136000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>33.572000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>98.212000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>9.0370000000000008</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>19.975999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>22.559000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>26.405999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>95.965000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>133.29599999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>71.753</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>41.109000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>22.853999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>27.902000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>21.027999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>37.171999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>31.257000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>40.438000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>46.311</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>94.135999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>14.025</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>15.596</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>33.198999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -5062,28 +5062,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3168" topLeftCell="A66" activePane="bottomLeft"/>
-      <selection activeCell="O2" sqref="O2"/>
-      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A25" activePane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>279.06976744186045</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>418.60465116279073</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>395.34883720930236</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>511.62790697674421</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>558.1395348837209</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>581.39534883720933</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>651.16279069767438</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>348.83720930232556</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>488.37209302325584</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>534.88372093023258</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>1.4229359211203001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>4.5519769090135398</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>6.9641670285147903</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>9.2473239917054801</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>9.9534090444337906</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>6.3154613715885803</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>9.1720363768313895</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>12.9463057989389</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>2.2831569631906898</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>6.8601740525742798</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>5.1720816259757898</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>1.9354451341071499</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>6.0251707067481197</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>9.2974565629968104</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -5788,7 +5788,7 @@
       <c r="D27" s="2"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="D28" s="2"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -5813,19 +5813,19 @@
       <c r="F29" s="1"/>
       <c r="H29">
         <f>L29+M29</f>
-        <v>382.14438342985062</v>
+        <v>86.654055199512641</v>
       </c>
       <c r="L29">
-        <v>272.10071530758057</v>
+        <v>61.700842473374294</v>
       </c>
       <c r="M29">
-        <v>110.04366812227003</v>
+        <v>24.953212726138339</v>
       </c>
       <c r="N29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -5836,19 +5836,19 @@
       <c r="F30" s="1"/>
       <c r="H30">
         <f t="shared" ref="H30:H51" si="4">L30+M30</f>
-        <v>1751.4978428322415</v>
+        <v>397.16504372613201</v>
       </c>
       <c r="L30">
-        <v>871.14849785407705</v>
+        <v>197.53934191702433</v>
       </c>
       <c r="M30">
-        <v>880.34934497816437</v>
+        <v>199.62570180910765</v>
       </c>
       <c r="N30">
-        <v>47.948497854077509</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>10.872675250357716</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -5859,19 +5859,19 @@
       <c r="F31" s="1"/>
       <c r="H31">
         <f t="shared" si="4"/>
-        <v>4171.4279338543429</v>
+        <v>945.9020258173116</v>
       </c>
       <c r="L31">
-        <v>1457.0174535050062</v>
+        <v>330.38944523923055</v>
       </c>
       <c r="M31">
-        <v>2714.4104803493365</v>
+        <v>615.51258057808104</v>
       </c>
       <c r="N31">
-        <v>333.34020028612167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>75.587347003655722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -5882,19 +5882,19 @@
       <c r="F32" s="1"/>
       <c r="H32">
         <f t="shared" si="4"/>
-        <v>5409.7355298586226</v>
+        <v>1226.6973990609129</v>
       </c>
       <c r="L32">
-        <v>971.30758226037051</v>
+        <v>220.25115243999338</v>
       </c>
       <c r="M32">
-        <v>4438.4279475982521</v>
+        <v>1006.4462466209194</v>
       </c>
       <c r="N32">
-        <v>500.90758226037059</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>113.58448577332669</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -5905,19 +5905,19 @@
       <c r="F33" s="1"/>
       <c r="H33">
         <f t="shared" si="4"/>
-        <v>7011.6153356947761</v>
+        <v>1589.935450270925</v>
       </c>
       <c r="L33">
-        <v>812.48869814020009</v>
+        <v>184.23780003179147</v>
       </c>
       <c r="M33">
-        <v>6199.1266375545765</v>
+        <v>1405.6976502391335</v>
       </c>
       <c r="N33">
-        <v>289.82203147353323</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>65.719281513272875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -5928,19 +5928,19 @@
       <c r="F34" s="1"/>
       <c r="H34">
         <f t="shared" si="4"/>
-        <v>4909.3007278020277</v>
+        <v>1113.2201196829999</v>
       </c>
       <c r="L34">
-        <v>287.46666666666687</v>
+        <v>65.185185185185247</v>
       </c>
       <c r="M34">
-        <v>4621.8340611353606</v>
+        <v>1048.0349344978147</v>
       </c>
       <c r="N34">
-        <v>182.93333333333328</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+        <v>41.481481481481481</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -5951,19 +5951,19 @@
       <c r="F35" s="1"/>
       <c r="H35">
         <f t="shared" si="4"/>
-        <v>272.12268646760583</v>
+        <v>61.705824595829014</v>
       </c>
       <c r="L35">
-        <v>195.6612399643173</v>
+        <v>44.367628109822533</v>
       </c>
       <c r="M35">
-        <v>76.461446503288556</v>
+        <v>17.338196486006478</v>
       </c>
       <c r="N35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -5974,19 +5974,19 @@
       <c r="F36" s="1"/>
       <c r="H36">
         <f t="shared" si="4"/>
-        <v>1466.848726400782</v>
+        <v>332.61875882103914</v>
       </c>
       <c r="L36">
-        <v>752.15655664585154</v>
+        <v>170.55704232332241</v>
       </c>
       <c r="M36">
-        <v>714.69216975493043</v>
+        <v>162.0617164977167</v>
       </c>
       <c r="N36">
-        <v>30.051293487956993</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>6.8143522648428574</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -5997,19 +5997,19 @@
       <c r="F37" s="1"/>
       <c r="H37">
         <f t="shared" si="4"/>
-        <v>3619.9403497752191</v>
+        <v>820.84815187646734</v>
       </c>
       <c r="L37">
-        <v>1282.9170383586077</v>
+        <v>290.91089305183857</v>
       </c>
       <c r="M37">
-        <v>2337.0233114166117</v>
+        <v>529.93725882462877</v>
       </c>
       <c r="N37">
-        <v>290.02230151650213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+        <v>65.764694221429068</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -6028,8 +6028,11 @@
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -6040,19 +6043,19 @@
       <c r="F39" s="1"/>
       <c r="H39">
         <f t="shared" si="4"/>
-        <v>729.44577132320444</v>
+        <v>165.40720438167909</v>
       </c>
       <c r="L39">
-        <v>459.89406779660811</v>
+        <v>104.28436911487717</v>
       </c>
       <c r="M39">
-        <v>269.55170352659633</v>
+        <v>61.122835266801914</v>
       </c>
       <c r="N39">
-        <v>21.473015165030727</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.8691644365149056</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -6063,19 +6066,19 @@
       <c r="F40" s="1"/>
       <c r="H40">
         <f t="shared" si="4"/>
-        <v>1376.630206197714</v>
+        <v>312.16104448927769</v>
       </c>
       <c r="L40">
-        <v>539.28412132024903</v>
+        <v>122.28664882545336</v>
       </c>
       <c r="M40">
-        <v>837.34608487746493</v>
+        <v>189.87439566382432</v>
       </c>
       <c r="N40">
-        <v>191.12622658340734</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+        <v>43.339280404400768</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -6086,19 +6089,19 @@
       <c r="F41" s="1"/>
       <c r="H41">
         <f t="shared" si="4"/>
-        <v>1427.1389813712315</v>
+        <v>323.61428149007526</v>
       </c>
       <c r="L41">
-        <v>232.15990187332525</v>
+        <v>52.643968678758576</v>
       </c>
       <c r="M41">
-        <v>1194.9790794979062</v>
+        <v>270.97031281131666</v>
       </c>
       <c r="N41">
-        <v>296.57894736841979</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+        <v>67.251461988303831</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -6109,10 +6112,10 @@
       <c r="F42" s="1"/>
       <c r="H42">
         <f t="shared" si="4"/>
-        <v>53.091847192281655</v>
+        <v>12.03896761729743</v>
       </c>
       <c r="L42">
-        <v>53.091847192281655</v>
+        <v>12.03896761729743</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -6121,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -6132,19 +6135,19 @@
       <c r="F43" s="1"/>
       <c r="H43">
         <f t="shared" si="4"/>
-        <v>789.47429580773655</v>
+        <v>179.01911469563191</v>
       </c>
       <c r="L43">
-        <v>385.9808460260781</v>
+        <v>87.524001366457625</v>
       </c>
       <c r="M43">
-        <v>403.49344978165851</v>
+        <v>91.495113329174302</v>
       </c>
       <c r="N43">
-        <v>29.610912817612764</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+        <v>6.7144927024065248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -6155,16 +6158,19 @@
       <c r="F44" s="1"/>
       <c r="H44">
         <f t="shared" si="4"/>
-        <v>329.06577502236286</v>
+        <v>74.618089574231959</v>
       </c>
       <c r="L44">
-        <v>182.34088419267016</v>
+        <v>41.347139272714337</v>
       </c>
       <c r="M44">
-        <v>146.7248908296927</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+        <v>33.27095030151763</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -6175,19 +6181,19 @@
       <c r="F45" s="1"/>
       <c r="H45">
         <f t="shared" si="4"/>
-        <v>1059.4950920623123</v>
+        <v>240.24832019553577</v>
       </c>
       <c r="L45">
-        <v>362.55186062126631</v>
+        <v>82.211306263325739</v>
       </c>
       <c r="M45">
-        <v>696.94323144104601</v>
+        <v>158.03701393221002</v>
       </c>
       <c r="N45">
-        <v>108.10580626921592</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+        <v>24.513788269663479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -6196,16 +6202,19 @@
       </c>
       <c r="H46">
         <f t="shared" si="4"/>
-        <v>465.19307600154139</v>
+        <v>105.48595827699356</v>
       </c>
       <c r="L46">
-        <v>171.74329434215599</v>
+        <v>38.944057673958291</v>
       </c>
       <c r="M46">
-        <v>293.44978165938539</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+        <v>66.541900603035259</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -6214,19 +6223,19 @@
       </c>
       <c r="H47">
         <f t="shared" si="4"/>
-        <v>934.50587059007205</v>
+        <v>211.90609310432478</v>
       </c>
       <c r="L47">
-        <v>237.56263914902607</v>
+        <v>53.869079172114773</v>
       </c>
       <c r="M47">
-        <v>696.94323144104601</v>
+        <v>158.03701393221002</v>
       </c>
       <c r="N47">
-        <v>84.832667773968865</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+        <v>19.236432601807003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -6235,16 +6244,19 @@
       </c>
       <c r="H48">
         <f t="shared" si="4"/>
-        <v>193.37506575989741</v>
+        <v>43.849221260747726</v>
       </c>
       <c r="L48">
-        <v>46.650174930204713</v>
+        <v>10.578270959230098</v>
       </c>
       <c r="M48">
-        <v>146.7248908296927</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+        <v>33.27095030151763</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -6253,19 +6265,19 @@
       </c>
       <c r="H49">
         <f t="shared" si="4"/>
-        <v>1107.1065983972544</v>
+        <v>251.04458013543194</v>
       </c>
       <c r="L49">
-        <v>226.75725341909006</v>
+        <v>51.418878326324297</v>
       </c>
       <c r="M49">
-        <v>880.34934497816437</v>
+        <v>199.62570180910765</v>
       </c>
       <c r="N49">
-        <v>61.351733399300393</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+        <v>13.911957686916193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -6274,19 +6286,22 @@
       </c>
       <c r="H50">
         <f t="shared" si="4"/>
-        <v>416.88578402543004</v>
+        <v>94.531923815290298</v>
       </c>
       <c r="L50">
-        <v>86.754779658621047</v>
+        <v>19.672285636875529</v>
       </c>
       <c r="M50">
-        <v>330.13100436680901</v>
+        <v>74.85963817841477</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
       </c>
       <c r="W50">
         <v>0.3</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -6295,16 +6310,16 @@
       </c>
       <c r="H51">
         <f t="shared" si="4"/>
-        <v>248.49292277654183</v>
+        <v>56.347601536630819</v>
       </c>
       <c r="L51">
-        <v>101.76803194684915</v>
+        <v>23.076651235113193</v>
       </c>
       <c r="M51">
-        <v>146.7248908296927</v>
+        <v>33.27095030151763</v>
       </c>
       <c r="N51">
-        <v>127.22302717602533</v>
+        <v>28.848758996831151</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -6314,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -6339,7 +6354,7 @@
         <v>0.45118836390597361</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -6358,7 +6373,7 @@
         <v>0.59343034025940078</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -6377,7 +6392,7 @@
         <v>0.69880578808779781</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -6402,7 +6417,7 @@
         <v>0.77686983985157021</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -6428,7 +6443,7 @@
         <v>0.83470111177841344</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -6451,7 +6466,7 @@
         <v>0.87754357174701814</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -6480,7 +6495,7 @@
         <v>0.90928204671058754</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -6503,7 +6518,7 @@
         <v>0.93279448726025027</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -6519,7 +6534,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -6541,7 +6556,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -6557,7 +6572,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -6573,7 +6588,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -6595,7 +6610,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -6611,7 +6626,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -6627,7 +6642,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -6649,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -6665,7 +6680,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -6681,7 +6696,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -6697,7 +6712,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -6719,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>43</v>
       </c>
@@ -6735,7 +6750,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -6751,7 +6766,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -6767,7 +6782,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -6789,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -6805,7 +6820,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -6821,7 +6836,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -6837,7 +6852,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -6859,7 +6874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -6875,7 +6890,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -6891,7 +6906,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>43</v>
       </c>
@@ -6907,7 +6922,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -6929,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -6945,7 +6960,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>43</v>
       </c>
@@ -6961,7 +6976,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -6977,7 +6992,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -6999,7 +7014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -7015,7 +7030,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>43</v>
       </c>
@@ -7031,7 +7046,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -7047,7 +7062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>43</v>
       </c>
@@ -7069,7 +7084,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>43</v>
       </c>
@@ -7085,7 +7100,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>43</v>
       </c>
@@ -7101,7 +7116,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>43</v>
       </c>
@@ -7117,7 +7132,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -7139,7 +7154,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>43</v>
       </c>
@@ -7155,7 +7170,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>43</v>
       </c>
@@ -7171,7 +7186,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>43</v>
       </c>
@@ -7193,7 +7208,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>43</v>
       </c>
@@ -7208,7 +7223,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -7223,28 +7238,28 @@
         <v>145</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
       <c r="J101" s="9"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="J102" s="11"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C103" s="9"/>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="J103" s="9"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C104" s="9"/>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
@@ -7252,7 +7267,7 @@
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
@@ -7275,13 +7290,13 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7310,7 +7325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -7330,7 +7345,7 @@
         <v>0.44370271473075212</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -7344,7 +7359,7 @@
       <c r="E3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -7358,7 +7373,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -7378,7 +7393,7 @@
         <v>0.48635162899911943</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -7392,7 +7407,7 @@
       <c r="E6" s="5"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -7406,7 +7421,7 @@
       <c r="E7" s="5"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -7426,7 +7441,7 @@
         <v>0.46170409104890797</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -7440,7 +7455,7 @@
       <c r="E9" s="5"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -7454,7 +7469,7 @@
       <c r="E10" s="5"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -7474,7 +7489,7 @@
         <v>0.47993147332354374</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -7488,7 +7503,7 @@
       <c r="E12" s="5"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -7502,7 +7517,7 @@
       <c r="E13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -7522,7 +7537,7 @@
         <v>0.45987654320987653</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -7536,7 +7551,7 @@
       <c r="E15" s="5"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -7550,7 +7565,7 @@
       <c r="E16" s="5"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -7570,7 +7585,7 @@
         <v>0.47866538338145653</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -7584,7 +7599,7 @@
       <c r="E18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -7598,7 +7613,7 @@
       <c r="E19" s="5"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -7618,7 +7633,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -7632,7 +7647,7 @@
       <c r="E21" s="5"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -7646,7 +7661,7 @@
       <c r="E22" s="5"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -7666,7 +7681,7 @@
         <v>0.46912050964431079</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -7680,7 +7695,7 @@
       <c r="E24" s="5"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -7694,7 +7709,7 @@
       <c r="E25" s="5"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -7714,7 +7729,7 @@
         <v>0.41360437842064107</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -7728,7 +7743,7 @@
       <c r="E27" s="5"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -7742,7 +7757,7 @@
       <c r="E28" s="5"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -7762,7 +7777,7 @@
         <v>0.47227694905713485</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -7776,7 +7791,7 @@
       <c r="E30" s="5"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -7790,7 +7805,7 @@
       <c r="E31" s="5"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -7810,7 +7825,7 @@
         <v>0.46190271201033145</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -7824,7 +7839,7 @@
       <c r="E33" s="5"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -7838,7 +7853,7 @@
       <c r="E34" s="5"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -7858,7 +7873,7 @@
         <v>0.47641093474426804</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -7872,7 +7887,7 @@
       <c r="E36" s="5"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -7886,7 +7901,7 @@
       <c r="E37" s="5"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -7909,7 +7924,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -7926,7 +7941,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -7943,7 +7958,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -7966,7 +7981,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -7983,7 +7998,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -8000,7 +8015,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -8023,7 +8038,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -8040,7 +8055,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -8057,7 +8072,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -8080,7 +8095,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -8097,7 +8112,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -8114,7 +8129,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -8137,7 +8152,7 @@
       </c>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -8154,7 +8169,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -8171,7 +8186,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -8194,7 +8209,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -8211,7 +8226,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -8228,7 +8243,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -8251,7 +8266,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -8268,7 +8283,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>41</v>
       </c>
@@ -8285,7 +8300,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -8308,7 +8323,7 @@
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -8325,7 +8340,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -8342,7 +8357,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -8372,7 +8387,7 @@
         <v>20.174684645498044</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>44</v>
       </c>
@@ -8402,7 +8417,7 @@
         <v>12.614615807812214</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -8432,7 +8447,7 @@
         <v>10.2986955631914</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -8462,7 +8477,7 @@
         <v>17.604570573283841</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -8492,7 +8507,7 @@
         <v>15.271238981895833</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -8522,7 +8537,7 @@
         <v>16.095937452239973</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -8552,7 +8567,7 @@
         <v>2.035973976272484</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>44</v>
       </c>
@@ -8582,7 +8597,7 @@
         <v>2.5177144580129656</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -8612,7 +8627,7 @@
         <v>3.6344693554527061</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -8642,7 +8657,7 @@
         <v>1.5039281705948373</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>45</v>
       </c>
@@ -8672,7 +8687,7 @@
         <v>0.6228534298709737</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -8702,7 +8717,7 @@
         <v>2.3476570213412313</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -8732,7 +8747,7 @@
         <v>3.5019110019110022</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>44</v>
       </c>
@@ -8762,7 +8777,7 @@
         <v>0.83741036991017592</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>41</v>
       </c>
@@ -8792,7 +8807,7 @@
         <v>1.0964912280701753</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -8822,7 +8837,7 @@
         <v>2.6534869662212337</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -8852,7 +8867,7 @@
         <v>2.4574192153589403</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -8882,7 +8897,7 @@
         <v>4.640211191760697</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -8912,7 +8927,7 @@
         <v>0.99663869496744473</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -8942,7 +8957,7 @@
         <v>0.59045570008321302</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -8972,7 +8987,7 @@
         <v>1.3078395330724735</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -9002,7 +9017,7 @@
         <v>3.1720933724576708</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -9032,7 +9047,7 @@
         <v>1.4356510784795695</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>43</v>
       </c>
@@ -9076,13 +9091,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9093,7 +9108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -9104,7 +9119,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -9115,7 +9130,7 @@
         <v>3922</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -9126,7 +9141,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -9137,7 +9152,7 @@
         <v>5302</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1997</v>
       </c>
@@ -9148,7 +9163,7 @@
         <v>3356</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1998</v>
       </c>
@@ -9159,7 +9174,7 @@
         <v>4322</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1999</v>
       </c>
@@ -9170,7 +9185,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2000</v>
       </c>
@@ -9181,7 +9196,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -9192,7 +9207,7 @@
         <v>5059</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -9216,13 +9231,13 @@
       <selection activeCell="A48" sqref="A47:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -9233,7 +9248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -9244,7 +9259,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -9255,7 +9270,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -9266,7 +9281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -9277,7 +9292,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9288,7 +9303,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9299,7 +9314,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -9310,7 +9325,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -9321,7 +9336,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -9332,7 +9347,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -9343,7 +9358,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -9354,7 +9369,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -9365,7 +9380,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -9376,7 +9391,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -9387,7 +9402,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -9398,7 +9413,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -9409,7 +9424,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -9420,7 +9435,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -9431,7 +9446,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -9442,7 +9457,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Cleaned up validation graphs etc
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/Observed.xlsx
+++ b/Prototypes/Gliricidia/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Gliricidia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E938A675-E279-4DED-8BBA-83E1578FD912}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B797C9B2-A4EA-43C8-A8D0-F4E6A5711587}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>Gliricidia.AboveGround.Wt</t>
   </si>
   <si>
-    <t>Hamakuapoko</t>
-  </si>
-  <si>
     <t>Gliricidia.Leaf.CoverGreen</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>HamakuapokoHarvestNil</t>
   </si>
 </sst>
 </file>
@@ -4252,7 +4252,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>34991</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4">
         <v>35049</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4">
         <v>35082</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4">
         <v>35118</v>
@@ -4320,7 +4320,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4">
         <v>35139</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4">
         <v>35174</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4">
         <v>35244</v>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4">
         <v>35307</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>35377</v>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4">
         <v>35409</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4">
         <v>35074</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4">
         <v>35460</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="4">
         <v>35489</v>
@@ -4451,7 +4451,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4">
         <v>35548</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="4">
         <v>35649</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4">
         <v>35754</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4">
         <v>34991</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4">
         <v>35049</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4">
         <v>35082</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4">
         <v>35118</v>
@@ -4547,7 +4547,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4">
         <v>35139</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4">
         <v>35174</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="4">
         <v>35244</v>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4">
         <v>35307</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4">
         <v>35377</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="4">
         <v>35409</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="4">
         <v>35074</v>
@@ -4645,7 +4645,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="4">
         <v>35460</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="4">
         <v>35489</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4">
         <v>35548</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="4">
         <v>35649</v>
@@ -4698,7 +4698,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4">
         <v>35754</v>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="4">
         <v>34991</v>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="4">
         <v>35049</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="4">
         <v>35082</v>
@@ -4750,7 +4750,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="4">
         <v>35118</v>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="4">
         <v>35139</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="4">
         <v>35174</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="4">
         <v>35244</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4">
         <v>35307</v>
@@ -4820,7 +4820,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="4">
         <v>35377</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="4">
         <v>35409</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="4">
         <v>35074</v>
@@ -4862,7 +4862,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="4">
         <v>35460</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="4">
         <v>35489</v>
@@ -4887,7 +4887,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="4">
         <v>35548</v>
@@ -4901,7 +4901,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="4">
         <v>35649</v>
@@ -4915,7 +4915,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="4">
         <v>35754</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="4">
         <v>34991</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="4">
         <v>35049</v>
@@ -4951,7 +4951,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B52" s="4">
         <v>35082</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53" s="4">
         <v>35118</v>
@@ -4979,7 +4979,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54" s="4">
         <v>35139</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55" s="4">
         <v>35174</v>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="4">
         <v>35244</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" s="4">
         <v>35307</v>
@@ -5035,7 +5035,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="4">
         <v>35377</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59" s="4">
         <v>35409</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60" s="4">
         <v>35074</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="4">
         <v>35460</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" s="4">
         <v>35489</v>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B63" s="4">
         <v>35548</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B64" s="4">
         <v>35649</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B65" s="4">
         <v>35754</v>
@@ -5152,7 +5152,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5178,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -5196,40 +5196,40 @@
         <v>28</v>
       </c>
       <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
       <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
-        <v>38</v>
-      </c>
       <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>53</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -5514,7 +5514,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B13">
         <f>YEAR(C13)</f>
@@ -5540,7 +5540,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B26" si="3">YEAR(C14)</f>
@@ -5566,7 +5566,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <f t="shared" si="3"/>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B16">
         <f t="shared" si="3"/>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <f t="shared" si="3"/>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <f t="shared" si="3"/>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B19">
         <f t="shared" si="3"/>
@@ -5696,7 +5696,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <f t="shared" si="3"/>
@@ -5722,7 +5722,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <f t="shared" si="3"/>
@@ -5745,7 +5745,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <f t="shared" si="3"/>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <f t="shared" si="3"/>
@@ -5791,7 +5791,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <f t="shared" si="3"/>
@@ -5814,7 +5814,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <f t="shared" si="3"/>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <f t="shared" si="3"/>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3">
         <v>35184</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3">
         <v>35236</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3">
         <v>35290</v>
@@ -5959,7 +5959,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="3">
         <v>35348</v>
@@ -5992,7 +5992,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="3">
         <v>35400</v>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3">
         <v>35461</v>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="3">
         <v>35520</v>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="3">
         <v>35184</v>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="3">
         <v>35236</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3">
         <v>35289</v>
@@ -6179,7 +6179,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="3">
         <v>35290</v>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="3">
         <v>35348</v>
@@ -6247,7 +6247,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="3">
         <v>35400</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="3">
         <v>35461</v>
@@ -6313,7 +6313,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="3">
         <v>35520</v>
@@ -6335,7 +6335,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="3">
         <v>35184</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3">
         <v>35235</v>
@@ -6401,7 +6401,7 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" s="3">
         <v>35236</v>
@@ -6436,7 +6436,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="3">
         <v>35290</v>
@@ -6469,7 +6469,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="3">
         <v>35291</v>
@@ -6502,7 +6502,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="3">
         <v>35347</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="3">
         <v>35348</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="3">
         <v>35399</v>
@@ -6597,7 +6597,7 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="3">
         <v>35400</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="3">
         <v>35461</v>
@@ -6671,7 +6671,7 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C52" s="3">
         <v>35520</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="3">
         <v>35215.666701388887</v>
@@ -6739,7 +6739,7 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="3">
         <v>35271.333402777775</v>
@@ -6780,7 +6780,7 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="3">
         <v>35327.000104166669</v>
@@ -6821,7 +6821,7 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="3">
         <v>35387.666805555556</v>
@@ -6862,7 +6862,7 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="3">
         <v>35439.333500000008</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3">
         <v>35499.000196759262</v>
@@ -6944,7 +6944,7 @@
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="3">
         <v>35520</v>
@@ -6975,7 +6975,7 @@
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="3">
         <v>35215.666701388887</v>
@@ -7009,7 +7009,7 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" s="3">
         <v>35271.333402777775</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C62" s="3">
         <v>35326.000100000005</v>
@@ -7083,7 +7083,7 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" s="3">
         <v>35327.000104166669</v>
@@ -7119,7 +7119,7 @@
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C64" s="3">
         <v>35387.666805555556</v>
@@ -7153,7 +7153,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" s="3">
         <v>35439.333500000008</v>
@@ -7187,7 +7187,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" s="3">
         <v>35499.000196759262</v>
@@ -7221,7 +7221,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67" s="3">
         <v>35520</v>
@@ -7241,7 +7241,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" s="3">
         <v>35215.667002314818</v>
@@ -7281,7 +7281,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C69" s="3">
         <v>35216.667002314818</v>
@@ -7317,7 +7317,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C70" s="3">
         <v>35271.334004629629</v>
@@ -7357,7 +7357,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C71" s="3">
         <v>35272.334004629629</v>
@@ -7393,7 +7393,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C72" s="3">
         <v>35326.001000000004</v>
@@ -7433,7 +7433,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="3">
         <v>35327.001000000004</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C74" s="3">
         <v>35387.667997685188</v>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C75" s="3">
         <v>35388.667997685188</v>
@@ -7545,7 +7545,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C76" s="3">
         <v>35439.335000000006</v>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="3">
         <v>35440.335000000006</v>
@@ -7621,7 +7621,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C78" s="3">
         <v>35499.002002314817</v>
@@ -7655,7 +7655,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C79" s="3">
         <v>35520</v>
@@ -7675,7 +7675,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C80" s="12">
         <v>33862</v>
@@ -7683,10 +7683,10 @@
       <c r="H80" s="2"/>
       <c r="M80" s="10"/>
       <c r="P80" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q80" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R80" s="10">
         <v>27</v>
@@ -7701,7 +7701,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C81" s="12">
         <v>33953</v>
@@ -7720,7 +7720,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C82" s="12">
         <v>34015</v>
@@ -7740,7 +7740,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C83" s="12">
         <v>34222</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C84" s="12">
         <v>34318</v>
@@ -7786,7 +7786,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C85" s="12">
         <v>34380</v>
@@ -7810,7 +7810,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C86" s="12">
         <v>34587</v>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C87" s="12">
         <v>34683</v>
@@ -7858,7 +7858,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C88" s="12">
         <v>34745</v>
@@ -7882,7 +7882,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C89" s="12">
         <v>34952</v>
@@ -7906,7 +7906,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C90" s="12">
         <v>35048</v>
@@ -7930,7 +7930,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C91" s="12">
         <v>35110</v>
@@ -7954,7 +7954,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C92" s="12">
         <v>35318</v>
@@ -7978,7 +7978,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C93" s="12">
         <v>35414</v>
@@ -8002,7 +8002,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C94" s="12">
         <v>35476</v>
@@ -8026,7 +8026,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C95" s="12">
         <v>35664</v>
@@ -8050,7 +8050,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C96" s="12">
         <v>35734</v>
@@ -8074,7 +8074,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C97" s="12">
         <v>35795</v>
@@ -8098,7 +8098,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C98" s="12">
         <v>35854</v>
@@ -8122,7 +8122,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C99" s="12">
         <v>36033</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C100" s="12">
         <v>36099</v>
@@ -8170,7 +8170,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C101" s="12">
         <v>36160</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C102" s="12">
         <v>36219</v>
@@ -8218,7 +8218,7 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C103" s="12">
         <v>36398</v>
@@ -8242,7 +8242,7 @@
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C104" s="12">
         <v>36464</v>
@@ -8266,7 +8266,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C105" s="12">
         <v>36525</v>
@@ -8290,7 +8290,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C106" s="12">
         <v>36584</v>
@@ -8314,7 +8314,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C107" s="12">
         <v>36764</v>
@@ -8338,7 +8338,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C108" s="12">
         <v>36830</v>
@@ -8362,7 +8362,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C109" s="12">
         <v>36891</v>
@@ -8386,7 +8386,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C110" s="12">
         <v>36950</v>
@@ -8410,7 +8410,7 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C111" s="12">
         <v>37129</v>
@@ -8434,7 +8434,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C112" s="12">
         <v>37195</v>
@@ -8459,7 +8459,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C113" s="12">
         <v>37256</v>
@@ -8484,7 +8484,7 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C114" s="12">
         <v>37315</v>
@@ -8509,7 +8509,7 @@
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C115" s="12">
         <v>37481</v>
@@ -8533,7 +8533,7 @@
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C116" s="12">
         <v>37560</v>
@@ -8557,7 +8557,7 @@
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C117" s="12">
         <v>37621</v>
@@ -8581,7 +8581,7 @@
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C118" s="12">
         <v>37680</v>
@@ -8605,7 +8605,7 @@
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C119" s="12">
         <v>37850</v>
@@ -8631,7 +8631,7 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C120" s="12">
         <v>37931</v>
@@ -8657,7 +8657,7 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C121" s="12">
         <v>37970</v>
@@ -8683,7 +8683,7 @@
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C122" s="12">
         <v>38018</v>
@@ -8709,7 +8709,7 @@
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C123" s="12">
         <v>38216</v>
@@ -8735,7 +8735,7 @@
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C124" s="12">
         <v>38341</v>
@@ -8761,7 +8761,7 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C125" s="12">
         <v>38383</v>
@@ -8787,7 +8787,7 @@
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C126" s="12">
         <v>38628</v>
@@ -8813,7 +8813,7 @@
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C127" s="12">
         <v>38690</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C128" s="12">
         <v>38740</v>
@@ -8901,21 +8901,21 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
       <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
         <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2">
         <v>1993</v>
@@ -8935,7 +8935,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>1993</v>
@@ -8949,7 +8949,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2">
         <v>1993</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2">
         <v>1993</v>
@@ -8983,7 +8983,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2">
         <v>1993</v>
@@ -8997,7 +8997,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2">
         <v>1993</v>
@@ -9011,7 +9011,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2">
         <v>1994</v>
@@ -9031,7 +9031,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2">
         <v>1994</v>
@@ -9045,7 +9045,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2">
         <v>1994</v>
@@ -9059,7 +9059,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2">
         <v>1994</v>
@@ -9079,7 +9079,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2">
         <v>1994</v>
@@ -9093,7 +9093,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2">
         <v>1994</v>
@@ -9107,7 +9107,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2">
         <v>1995</v>
@@ -9127,7 +9127,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2">
         <v>1995</v>
@@ -9141,7 +9141,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2">
         <v>1995</v>
@@ -9155,7 +9155,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2">
         <v>1995</v>
@@ -9175,7 +9175,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2">
         <v>1995</v>
@@ -9189,7 +9189,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2">
         <v>1995</v>
@@ -9203,7 +9203,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2">
         <v>1996</v>
@@ -9223,7 +9223,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2">
         <v>1996</v>
@@ -9237,7 +9237,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2">
         <v>1996</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2">
         <v>1996</v>
@@ -9271,7 +9271,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2">
         <v>1996</v>
@@ -9285,7 +9285,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2">
         <v>1996</v>
@@ -9299,7 +9299,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2">
         <v>1997</v>
@@ -9319,7 +9319,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2">
         <v>1997</v>
@@ -9333,7 +9333,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2">
         <v>1997</v>
@@ -9347,7 +9347,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2">
         <v>1997</v>
@@ -9367,7 +9367,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2">
         <v>1997</v>
@@ -9381,7 +9381,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2">
         <v>1997</v>
@@ -9395,7 +9395,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2">
         <v>1998</v>
@@ -9415,7 +9415,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="2">
         <v>1998</v>
@@ -9429,7 +9429,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
         <v>1998</v>
@@ -9443,7 +9443,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2">
         <v>1998</v>
@@ -9463,7 +9463,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="2">
         <v>1998</v>
@@ -9477,7 +9477,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2">
         <v>1998</v>
@@ -9491,7 +9491,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
         <v>1999</v>
@@ -9514,7 +9514,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2">
         <v>1999</v>
@@ -9531,7 +9531,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2">
         <v>1999</v>
@@ -9548,7 +9548,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2">
         <v>1999</v>
@@ -9571,7 +9571,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2">
         <v>1999</v>
@@ -9588,7 +9588,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>1999</v>
@@ -9605,7 +9605,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2">
         <v>2000</v>
@@ -9628,7 +9628,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2">
         <v>2000</v>
@@ -9645,7 +9645,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="2">
         <v>2000</v>
@@ -9662,7 +9662,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2">
         <v>2000</v>
@@ -9685,7 +9685,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="2">
         <v>2000</v>
@@ -9702,7 +9702,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2">
         <v>2000</v>
@@ -9719,7 +9719,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" s="2">
         <v>2001</v>
@@ -9742,7 +9742,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="2">
         <v>2001</v>
@@ -9759,7 +9759,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B52" s="2">
         <v>2001</v>
@@ -9776,7 +9776,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B53" s="2">
         <v>2001</v>
@@ -9799,7 +9799,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="2">
         <v>2001</v>
@@ -9816,7 +9816,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2">
         <v>2001</v>
@@ -9833,7 +9833,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="2">
         <v>2002</v>
@@ -9856,7 +9856,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2">
         <v>2002</v>
@@ -9873,7 +9873,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="2">
         <v>2002</v>
@@ -9890,7 +9890,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" s="2">
         <v>2002</v>
@@ -9913,7 +9913,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="2">
         <v>2002</v>
@@ -9930,7 +9930,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2">
         <v>2002</v>
@@ -9947,7 +9947,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" s="2">
         <v>2003</v>
@@ -9977,7 +9977,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="2">
         <v>2003</v>
@@ -10007,7 +10007,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" s="2">
         <v>2003</v>
@@ -10037,7 +10037,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65" s="2">
         <v>2003</v>
@@ -10067,7 +10067,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B66" s="2">
         <v>2003</v>
@@ -10097,7 +10097,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B67" s="2">
         <v>2003</v>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B68" s="2">
         <v>2004</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69" s="2">
         <v>2004</v>
@@ -10187,7 +10187,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B70" s="2">
         <v>2004</v>
@@ -10217,7 +10217,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B71" s="2">
         <v>2004</v>
@@ -10247,7 +10247,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" s="2">
         <v>2004</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B73" s="2">
         <v>2004</v>
@@ -10307,7 +10307,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" s="2">
         <v>2005</v>
@@ -10337,7 +10337,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B75" s="2">
         <v>2005</v>
@@ -10367,7 +10367,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B76" s="2">
         <v>2005</v>
@@ -10397,7 +10397,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B77" s="2">
         <v>2005</v>
@@ -10427,7 +10427,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B78" s="2">
         <v>2005</v>
@@ -10457,7 +10457,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="2">
         <v>2005</v>
@@ -10487,7 +10487,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B80" s="2">
         <v>2006</v>
@@ -10517,7 +10517,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="2">
         <v>2006</v>
@@ -10547,7 +10547,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B82" s="2">
         <v>2006</v>
@@ -10577,7 +10577,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B83" s="2">
         <v>2006</v>
@@ -10607,7 +10607,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84" s="2">
         <v>2006</v>
@@ -10637,7 +10637,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B85" s="2">
         <v>2006</v>

</xml_diff>